<commit_message>
Changing chart layout in result Excel.
</commit_message>
<xml_diff>
--- a/results/gdb_benchmark_results.xlsx
+++ b/results/gdb_benchmark_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandizi/Documents/Work/RRes/events/2018_swat4ls/paper/graphdb-benchmarks/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CBBAD7-3455-8444-95CF-A46A1FCACD8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84836C0B-049A-9847-911B-7436A3E0E54D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -447,9 +447,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -461,6 +458,9 @@
     </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1271,7 +1271,9 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="0432FF"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -1443,7 +1445,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="narHorz">
+            <a:pattFill prst="dkDnDiag">
               <a:fgClr>
                 <a:srgbClr val="FF0000"/>
               </a:fgClr>
@@ -1452,7 +1454,9 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -1633,7 +1637,9 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="0432FF"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -1805,7 +1811,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="narHorz">
+            <a:pattFill prst="dkDnDiag">
               <a:fgClr>
                 <a:srgbClr val="FF0000"/>
               </a:fgClr>
@@ -1814,7 +1820,9 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -1995,7 +2003,9 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="0432FF"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -2167,7 +2177,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="narHorz">
+            <a:pattFill prst="dkDnDiag">
               <a:fgClr>
                 <a:srgbClr val="FF0000"/>
               </a:fgClr>
@@ -2176,7 +2186,9 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -4824,15 +4836,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -5297,15 +5309,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -5755,7 +5767,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B6:B8"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5767,15 +5779,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -6238,7 +6250,7 @@
       <c r="B1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>47</v>
       </c>
       <c r="D1" s="25" t="s">
@@ -6297,12 +6309,12 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="26" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="26" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6317,8 +6329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CD3143-BDBF-FD41-9A6E-2395CA27F127}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6326,661 +6338,661 @@
     <col min="1" max="7" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="28" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:7" s="27" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="27" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="29" t="str">
+      <c r="A2" s="28" t="str">
         <f>Biopax!$A9</f>
         <v>cnt</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="29">
         <f>Biopax!$C9</f>
         <v>4.9505E-2</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="29">
         <f>Biopax!$D9</f>
         <v>622.47959200000003</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="29">
         <f>Ara!$C9</f>
         <v>0.47169800000000001</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="29">
         <f>Ara!$D9</f>
         <v>5543.3195880000003</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="29">
         <f>Wheat!$C9</f>
         <v>0.70454499999999998</v>
       </c>
-      <c r="G2" s="30">
+      <c r="G2" s="29">
         <f>Wheat!$D9</f>
         <v>14721.444444000001</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="29" t="str">
+      <c r="A3" s="28" t="str">
         <f>Biopax!$A10</f>
         <v>cntType</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="29">
         <f>Biopax!$C10</f>
         <v>0.76</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="29">
         <f>Biopax!$D10</f>
         <v>2.548387</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <f>Ara!$C10</f>
         <v>5.7818180000000003</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="29">
         <f>Ara!$D10</f>
         <v>5.0206189999999999</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="29">
         <f>Wheat!$C10</f>
         <v>6.5729170000000003</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="29">
         <f>Wheat!$D10</f>
         <v>13.847826</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="29" t="str">
+      <c r="A4" s="28" t="str">
         <f>Biopax!$A11</f>
         <v>cntRel</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="29">
         <f>Biopax!$C11</f>
         <v>0.114286</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="29">
         <f>Biopax!$D11</f>
         <v>64.877778000000006</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="29">
         <f>Ara!$C11</f>
         <v>0.36274499999999998</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="29">
         <f>Ara!$D11</f>
         <v>546.69662900000003</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="29">
         <f>Wheat!$C11</f>
         <v>0.655914</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="29">
         <f>Wheat!$D11</f>
         <v>1401.9534880000001</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="29" t="str">
+      <c r="A5" s="28" t="str">
         <f>Biopax!$A12</f>
         <v>cntRelType</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="29">
         <f>Biopax!$C12</f>
         <v>1.6727270000000001</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="29">
         <f>Biopax!$D12</f>
         <v>34.025641</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="29">
         <f>Ara!$C12</f>
         <v>6.8738739999999998</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <f>Ara!$D12</f>
         <v>92.782608999999994</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="29">
         <f>Wheat!$C12</f>
         <v>8</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="29">
         <f>Wheat!$D12</f>
         <v>100.835052</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A6" s="29" t="str">
+      <c r="A6" s="28" t="str">
         <f>Biopax!$A13</f>
         <v>sel</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="29">
         <f>Biopax!$C13</f>
         <v>0.31428600000000001</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="29">
         <f>Biopax!$D13</f>
         <v>6.1818179999999998</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="29">
         <f>Ara!$C13</f>
         <v>0.76087000000000005</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="29">
         <f>Ara!$D13</f>
         <v>4.6306310000000002</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="29">
         <f>Wheat!$C13</f>
         <v>1.605769</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="29">
         <f>Wheat!$D13</f>
         <v>6.9036140000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="29" t="str">
+      <c r="A7" s="28" t="str">
         <f>Biopax!$A14</f>
         <v>join</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="29">
         <f>Biopax!$C14</f>
         <v>1.0659339999999999</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="29">
         <f>Biopax!$D14</f>
         <v>8.6190479999999994</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="29">
         <f>Ara!$C14</f>
         <v>1.448</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <f>Ara!$D14</f>
         <v>9.0099009999999993</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="29">
         <f>Wheat!$C14</f>
         <v>1.535088</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="29">
         <f>Wheat!$D14</f>
         <v>9.8627450000000003</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="29" t="str">
+      <c r="A8" s="28" t="str">
         <f>Biopax!$A15</f>
         <v>joinRel</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="29">
         <f>Biopax!$C15</f>
         <v>1.194175</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="29">
         <f>Biopax!$D15</f>
         <v>13.4</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="29">
         <f>Ara!$C15</f>
         <v>1.8658539999999999</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="29">
         <f>Ara!$D15</f>
         <v>17.393162</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="29">
         <f>Wheat!$C15</f>
         <v>4.68</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="29">
         <f>Wheat!$D15</f>
         <v>21.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="29" t="str">
+      <c r="A9" s="28" t="str">
         <f>Biopax!$A16</f>
         <v>joinFilter</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="29">
         <f>Biopax!$C16</f>
         <v>3.7083330000000001</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="29">
         <f>Biopax!$D16</f>
         <v>9.5775860000000002</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="29">
         <f>Ara!$C16</f>
         <v>8.7522120000000001</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <f>Ara!$D16</f>
         <v>10.4</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="29">
         <f>Wheat!$C16</f>
         <v>9.4180329999999994</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="29">
         <f>Wheat!$D16</f>
         <v>10.657895</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="29" t="str">
+      <c r="A10" s="28" t="str">
         <f>Biopax!$A17</f>
         <v>joinRe</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="29">
         <f>Biopax!$C17</f>
         <v>3.913043</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="29">
         <f>Biopax!$D17</f>
         <v>10.494624</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="29">
         <f>Ara!$C17</f>
         <v>5.8192769999999996</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="29">
         <f>Ara!$D17</f>
         <v>18.807338999999999</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="29">
         <f>Wheat!$C17</f>
         <v>5.9545450000000004</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="29">
         <f>Wheat!$D17</f>
         <v>10.666667</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="29" t="str">
+      <c r="A11" s="28" t="str">
         <f>Biopax!$A18</f>
         <v>joinReif</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="29">
         <f>Biopax!$C18</f>
         <v>6.8415840000000001</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="29">
         <f>Biopax!$D18</f>
         <v>373.79411800000003</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="29">
         <f>Ara!$C18</f>
         <v>491.942857</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="29">
         <f>Ara!$D18</f>
         <v>60.181818</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="29">
         <f>Wheat!$C18</f>
         <v>14.741935</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11" s="29">
         <f>Wheat!$D18</f>
         <v>66.676190000000005</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A12" s="29" t="str">
+      <c r="A12" s="28" t="str">
         <f>Biopax!$A19</f>
         <v>varPathC</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="29">
         <f>Biopax!$C19</f>
         <v>0.61904800000000004</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="29">
         <f>Biopax!$D19</f>
         <v>27.914894</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="29">
         <f>Ara!$C19</f>
         <v>1.8921570000000001</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <f>Ara!$D19</f>
         <v>25.590909</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="29">
         <f>Wheat!$C19</f>
         <v>1.81</v>
       </c>
-      <c r="G12" s="30">
+      <c r="G12" s="29">
         <f>Wheat!$D19</f>
         <v>25.862745</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A13" s="29" t="str">
+      <c r="A13" s="28" t="str">
         <f>Biopax!$A20</f>
         <v>varPath</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="29">
         <f>Biopax!$C20</f>
         <v>5.1397849999999998</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="29">
         <f>Biopax!$D20</f>
         <v>89.483146000000005</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="29">
         <f>Ara!$C20</f>
         <v>7.5833329999999997</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="29">
         <f>Ara!$D20</f>
         <v>18.135922000000001</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="29">
         <f>Wheat!$C20</f>
         <v>4.0416670000000003</v>
       </c>
-      <c r="G13" s="30">
+      <c r="G13" s="29">
         <f>Wheat!$D20</f>
         <v>33.349592999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="29" t="str">
+      <c r="A14" s="28" t="str">
         <f>Biopax!$A21</f>
         <v>2union</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="29">
         <f>Biopax!$C21</f>
         <v>11.172043</v>
       </c>
-      <c r="C14" s="30">
+      <c r="C14" s="29">
         <f>Biopax!$D21</f>
         <v>12.308510999999999</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="29">
         <f>Ara!$C21</f>
         <v>10.340206</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="29">
         <f>Ara!$D21</f>
         <v>12.383838000000001</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="29">
         <f>Wheat!$C21</f>
         <v>12.25</v>
       </c>
-      <c r="G14" s="30">
+      <c r="G14" s="29">
         <f>Wheat!$D21</f>
         <v>19.73</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="29" t="str">
+      <c r="A15" s="28" t="str">
         <f>Biopax!$A22</f>
         <v>2union1Nest</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="29">
         <f>Biopax!$C22</f>
         <v>30.958333</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="29">
         <f>Biopax!$D22</f>
         <v>11.049020000000001</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="29">
         <f>Ara!$C22</f>
         <v>44.315789000000002</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="29">
         <f>Ara!$D22</f>
         <v>11.75</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="29">
         <f>Wheat!$C22</f>
         <v>41.304761999999997</v>
       </c>
-      <c r="G15" s="30">
+      <c r="G15" s="29">
         <f>Wheat!$D22</f>
         <v>11.644231</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A16" s="29" t="str">
+      <c r="A16" s="28" t="str">
         <f>Biopax!$A23</f>
         <v>pway</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="29">
         <f>Biopax!$C23</f>
         <v>4.9519229999999999</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="29">
         <f>Biopax!$D23</f>
         <v>38.512605000000001</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="29">
         <f>Ara!$C23</f>
         <v>11.361905</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="29">
         <f>Ara!$D23</f>
         <v>36.090909000000003</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="29">
         <f>Wheat!$C23</f>
         <v>8.3406590000000005</v>
       </c>
-      <c r="G16" s="30">
+      <c r="G16" s="29">
         <f>Wheat!$D23</f>
         <v>34.221238999999997</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A17" s="29" t="str">
+      <c r="A17" s="28" t="str">
         <f>Biopax!$A24</f>
         <v>grp</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="29">
         <f>Biopax!$C24</f>
         <v>8.9894739999999995</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="29">
         <f>Biopax!$D24</f>
         <v>21.039216</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="29">
         <f>Ara!$C24</f>
         <v>13.53012</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="29">
         <f>Ara!$D24</f>
         <v>26.521277000000001</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="29">
         <f>Wheat!$C24</f>
         <v>14.344086000000001</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G17" s="29">
         <f>Wheat!$D24</f>
         <v>23.847826000000001</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A18" s="29" t="str">
+      <c r="A18" s="28" t="str">
         <f>Biopax!$A25</f>
         <v>grpAg</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="29">
         <f>Biopax!$C25</f>
         <v>10.757009</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="29">
         <f>Biopax!$D25</f>
         <v>23.666667</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="29">
         <f>Ara!$C25</f>
         <v>19.221239000000001</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="29">
         <f>Ara!$D25</f>
         <v>30.169643000000001</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="29">
         <f>Wheat!$C25</f>
         <v>18.600000000000001</v>
       </c>
-      <c r="G18" s="30">
+      <c r="G18" s="29">
         <f>Wheat!$D25</f>
         <v>27.177569999999999</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A19" s="29" t="str">
+      <c r="A19" s="28" t="str">
         <f>Biopax!$A26</f>
         <v>mulGrpAg</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="29">
         <f>Biopax!$C26</f>
         <v>827</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="29">
         <f>Biopax!$D26</f>
         <v>65.769912000000005</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="29">
         <f>Ara!$C26</f>
         <v>753.010989</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="29">
         <f>Ara!$D26</f>
         <v>83.12</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="29">
         <f>Wheat!$C26</f>
         <v>780.01851899999997</v>
       </c>
-      <c r="G19" s="30">
+      <c r="G19" s="29">
         <f>Wheat!$D26</f>
         <v>56.32</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A20" s="29" t="str">
+      <c r="A20" s="28" t="str">
         <f>Biopax!$A27</f>
         <v>nestAg</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B20" s="29">
         <f>Biopax!$C27</f>
         <v>10.677083</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="29">
         <f>Biopax!$D27</f>
         <v>22.274509999999999</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="29">
         <f>Ara!$C27</f>
         <v>20.428571000000002</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="29">
         <f>Ara!$D27</f>
         <v>26.955752</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="29">
         <f>Wheat!$C27</f>
         <v>19.745097999999999</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="29">
         <f>Wheat!$D27</f>
         <v>24.944444000000001</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A21" s="29" t="str">
+      <c r="A21" s="28" t="str">
         <f>Biopax!$A28</f>
         <v>exist</v>
       </c>
-      <c r="B21" s="30">
+      <c r="B21" s="29">
         <f>Biopax!$C28</f>
         <v>31.053763</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="29">
         <f>Biopax!$D28</f>
         <v>30.904254999999999</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="29">
         <f>Ara!$C28</f>
         <v>21.775281</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="29">
         <f>Ara!$D28</f>
         <v>36.989691000000001</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="29">
         <f>Wheat!$C28</f>
         <v>19.142856999999999</v>
       </c>
-      <c r="G21" s="30">
+      <c r="G21" s="29">
         <f>Wheat!$D28</f>
         <v>34.734693999999998</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A22" s="29" t="str">
+      <c r="A22" s="28" t="str">
         <f>Biopax!$A29</f>
         <v>existAg</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="29">
         <f>Biopax!$C29</f>
         <v>59.613208</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="29">
         <f>Biopax!$D29</f>
         <v>51.344828</v>
       </c>
-      <c r="D22" s="30">
+      <c r="D22" s="29">
         <f>Ara!$C29</f>
         <v>25.355768999999999</v>
       </c>
-      <c r="E22" s="30">
+      <c r="E22" s="29">
         <f>Ara!$D29</f>
         <v>62.617283999999998</v>
       </c>
-      <c r="F22" s="30">
+      <c r="F22" s="29">
         <f>Wheat!$C29</f>
         <v>36.047618999999997</v>
       </c>
-      <c r="G22" s="30">
+      <c r="G22" s="29">
         <f>Wheat!$D29</f>
         <v>59.063063</v>
       </c>
     </row>
     <row r="50" spans="3:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="C50" s="27" t="s">
+      <c r="C50" s="26" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor addition to README. Minor improvements to the results xls.
</commit_message>
<xml_diff>
--- a/results/gdb_benchmark_results.xlsx
+++ b/results/gdb_benchmark_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandizi/Documents/Work/RRes/events/2018_swat4ls/paper/graphdb-benchmarks/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84836C0B-049A-9847-911B-7436A3E0E54D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982F210C-75DF-5D47-AABF-C6DF29966479}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,7 +196,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -228,8 +228,21 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,8 +261,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3700"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF007CFE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -362,13 +387,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -453,14 +493,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,7 +588,15 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFFFFFFF"/>
+      <color rgb="FFF0EEF1"/>
+      <color rgb="FFD5D4D4"/>
+      <color rgb="FFE0E0E0"/>
+      <color rgb="FFE7E5E8"/>
+      <color rgb="FF007CFE"/>
       <color rgb="FF0432FF"/>
+      <color rgb="FFFF3700"/>
+      <color rgb="FFFF5400"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3709,15 +3769,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>173627</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>122827</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>300182</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>126999</xdr:rowOff>
+      <xdr:colOff>249382</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>63499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4823,7 +4883,7 @@
   <dimension ref="A1:IV29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
@@ -4836,15 +4896,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -5309,15 +5369,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -5779,15 +5839,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -6329,8 +6389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CD3143-BDBF-FD41-9A6E-2395CA27F127}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6339,654 +6399,654 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="27" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="32" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="28" t="str">
+      <c r="A2" s="30" t="str">
         <f>Biopax!$A9</f>
         <v>cnt</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="33">
         <f>Biopax!$C9</f>
         <v>4.9505E-2</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="34">
         <f>Biopax!$D9</f>
         <v>622.47959200000003</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="33">
         <f>Ara!$C9</f>
         <v>0.47169800000000001</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="34">
         <f>Ara!$D9</f>
         <v>5543.3195880000003</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="33">
         <f>Wheat!$C9</f>
         <v>0.70454499999999998</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="34">
         <f>Wheat!$D9</f>
         <v>14721.444444000001</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="28" t="str">
+      <c r="A3" s="30" t="str">
         <f>Biopax!$A10</f>
         <v>cntType</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="33">
         <f>Biopax!$C10</f>
         <v>0.76</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="34">
         <f>Biopax!$D10</f>
         <v>2.548387</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="33">
         <f>Ara!$C10</f>
         <v>5.7818180000000003</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="34">
         <f>Ara!$D10</f>
         <v>5.0206189999999999</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="33">
         <f>Wheat!$C10</f>
         <v>6.5729170000000003</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="34">
         <f>Wheat!$D10</f>
         <v>13.847826</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="28" t="str">
+      <c r="A4" s="30" t="str">
         <f>Biopax!$A11</f>
         <v>cntRel</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="33">
         <f>Biopax!$C11</f>
         <v>0.114286</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="34">
         <f>Biopax!$D11</f>
         <v>64.877778000000006</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="33">
         <f>Ara!$C11</f>
         <v>0.36274499999999998</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="34">
         <f>Ara!$D11</f>
         <v>546.69662900000003</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="33">
         <f>Wheat!$C11</f>
         <v>0.655914</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="34">
         <f>Wheat!$D11</f>
         <v>1401.9534880000001</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="28" t="str">
+      <c r="A5" s="30" t="str">
         <f>Biopax!$A12</f>
         <v>cntRelType</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="33">
         <f>Biopax!$C12</f>
         <v>1.6727270000000001</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="34">
         <f>Biopax!$D12</f>
         <v>34.025641</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="33">
         <f>Ara!$C12</f>
         <v>6.8738739999999998</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="34">
         <f>Ara!$D12</f>
         <v>92.782608999999994</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="33">
         <f>Wheat!$C12</f>
         <v>8</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="34">
         <f>Wheat!$D12</f>
         <v>100.835052</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A6" s="28" t="str">
+      <c r="A6" s="30" t="str">
         <f>Biopax!$A13</f>
         <v>sel</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="33">
         <f>Biopax!$C13</f>
         <v>0.31428600000000001</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="34">
         <f>Biopax!$D13</f>
         <v>6.1818179999999998</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="33">
         <f>Ara!$C13</f>
         <v>0.76087000000000005</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="34">
         <f>Ara!$D13</f>
         <v>4.6306310000000002</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="33">
         <f>Wheat!$C13</f>
         <v>1.605769</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="34">
         <f>Wheat!$D13</f>
         <v>6.9036140000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="28" t="str">
+      <c r="A7" s="30" t="str">
         <f>Biopax!$A14</f>
         <v>join</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="33">
         <f>Biopax!$C14</f>
         <v>1.0659339999999999</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="34">
         <f>Biopax!$D14</f>
         <v>8.6190479999999994</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="33">
         <f>Ara!$C14</f>
         <v>1.448</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="34">
         <f>Ara!$D14</f>
         <v>9.0099009999999993</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="33">
         <f>Wheat!$C14</f>
         <v>1.535088</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="34">
         <f>Wheat!$D14</f>
         <v>9.8627450000000003</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="28" t="str">
+      <c r="A8" s="30" t="str">
         <f>Biopax!$A15</f>
         <v>joinRel</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="33">
         <f>Biopax!$C15</f>
         <v>1.194175</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="34">
         <f>Biopax!$D15</f>
         <v>13.4</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="33">
         <f>Ara!$C15</f>
         <v>1.8658539999999999</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="34">
         <f>Ara!$D15</f>
         <v>17.393162</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="33">
         <f>Wheat!$C15</f>
         <v>4.68</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="34">
         <f>Wheat!$D15</f>
         <v>21.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="28" t="str">
+      <c r="A9" s="30" t="str">
         <f>Biopax!$A16</f>
         <v>joinFilter</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="33">
         <f>Biopax!$C16</f>
         <v>3.7083330000000001</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="34">
         <f>Biopax!$D16</f>
         <v>9.5775860000000002</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="33">
         <f>Ara!$C16</f>
         <v>8.7522120000000001</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="34">
         <f>Ara!$D16</f>
         <v>10.4</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="33">
         <f>Wheat!$C16</f>
         <v>9.4180329999999994</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="34">
         <f>Wheat!$D16</f>
         <v>10.657895</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="28" t="str">
+      <c r="A10" s="30" t="str">
         <f>Biopax!$A17</f>
         <v>joinRe</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="33">
         <f>Biopax!$C17</f>
         <v>3.913043</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="34">
         <f>Biopax!$D17</f>
         <v>10.494624</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="33">
         <f>Ara!$C17</f>
         <v>5.8192769999999996</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="34">
         <f>Ara!$D17</f>
         <v>18.807338999999999</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="33">
         <f>Wheat!$C17</f>
         <v>5.9545450000000004</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="34">
         <f>Wheat!$D17</f>
         <v>10.666667</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="28" t="str">
+      <c r="A11" s="30" t="str">
         <f>Biopax!$A18</f>
         <v>joinReif</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="33">
         <f>Biopax!$C18</f>
         <v>6.8415840000000001</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="34">
         <f>Biopax!$D18</f>
         <v>373.79411800000003</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="33">
         <f>Ara!$C18</f>
         <v>491.942857</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="34">
         <f>Ara!$D18</f>
         <v>60.181818</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="33">
         <f>Wheat!$C18</f>
         <v>14.741935</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="34">
         <f>Wheat!$D18</f>
         <v>66.676190000000005</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A12" s="28" t="str">
+      <c r="A12" s="30" t="str">
         <f>Biopax!$A19</f>
         <v>varPathC</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="33">
         <f>Biopax!$C19</f>
         <v>0.61904800000000004</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="34">
         <f>Biopax!$D19</f>
         <v>27.914894</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="33">
         <f>Ara!$C19</f>
         <v>1.8921570000000001</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="34">
         <f>Ara!$D19</f>
         <v>25.590909</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="33">
         <f>Wheat!$C19</f>
         <v>1.81</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="34">
         <f>Wheat!$D19</f>
         <v>25.862745</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A13" s="28" t="str">
+      <c r="A13" s="30" t="str">
         <f>Biopax!$A20</f>
         <v>varPath</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="33">
         <f>Biopax!$C20</f>
         <v>5.1397849999999998</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="34">
         <f>Biopax!$D20</f>
         <v>89.483146000000005</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="33">
         <f>Ara!$C20</f>
         <v>7.5833329999999997</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="34">
         <f>Ara!$D20</f>
         <v>18.135922000000001</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="33">
         <f>Wheat!$C20</f>
         <v>4.0416670000000003</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="34">
         <f>Wheat!$D20</f>
         <v>33.349592999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="28" t="str">
+      <c r="A14" s="30" t="str">
         <f>Biopax!$A21</f>
         <v>2union</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="33">
         <f>Biopax!$C21</f>
         <v>11.172043</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="34">
         <f>Biopax!$D21</f>
         <v>12.308510999999999</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="33">
         <f>Ara!$C21</f>
         <v>10.340206</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="34">
         <f>Ara!$D21</f>
         <v>12.383838000000001</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="33">
         <f>Wheat!$C21</f>
         <v>12.25</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="34">
         <f>Wheat!$D21</f>
         <v>19.73</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="28" t="str">
+      <c r="A15" s="30" t="str">
         <f>Biopax!$A22</f>
         <v>2union1Nest</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="33">
         <f>Biopax!$C22</f>
         <v>30.958333</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="34">
         <f>Biopax!$D22</f>
         <v>11.049020000000001</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="33">
         <f>Ara!$C22</f>
         <v>44.315789000000002</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="34">
         <f>Ara!$D22</f>
         <v>11.75</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="33">
         <f>Wheat!$C22</f>
         <v>41.304761999999997</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="34">
         <f>Wheat!$D22</f>
         <v>11.644231</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A16" s="28" t="str">
+      <c r="A16" s="30" t="str">
         <f>Biopax!$A23</f>
         <v>pway</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="33">
         <f>Biopax!$C23</f>
         <v>4.9519229999999999</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="34">
         <f>Biopax!$D23</f>
         <v>38.512605000000001</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="33">
         <f>Ara!$C23</f>
         <v>11.361905</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="34">
         <f>Ara!$D23</f>
         <v>36.090909000000003</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="33">
         <f>Wheat!$C23</f>
         <v>8.3406590000000005</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="34">
         <f>Wheat!$D23</f>
         <v>34.221238999999997</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A17" s="28" t="str">
+      <c r="A17" s="30" t="str">
         <f>Biopax!$A24</f>
         <v>grp</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="33">
         <f>Biopax!$C24</f>
         <v>8.9894739999999995</v>
       </c>
-      <c r="C17" s="29">
+      <c r="C17" s="34">
         <f>Biopax!$D24</f>
         <v>21.039216</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="33">
         <f>Ara!$C24</f>
         <v>13.53012</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="34">
         <f>Ara!$D24</f>
         <v>26.521277000000001</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="33">
         <f>Wheat!$C24</f>
         <v>14.344086000000001</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="34">
         <f>Wheat!$D24</f>
         <v>23.847826000000001</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A18" s="28" t="str">
+      <c r="A18" s="30" t="str">
         <f>Biopax!$A25</f>
         <v>grpAg</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="33">
         <f>Biopax!$C25</f>
         <v>10.757009</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C18" s="34">
         <f>Biopax!$D25</f>
         <v>23.666667</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="33">
         <f>Ara!$C25</f>
         <v>19.221239000000001</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="34">
         <f>Ara!$D25</f>
         <v>30.169643000000001</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="33">
         <f>Wheat!$C25</f>
         <v>18.600000000000001</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="34">
         <f>Wheat!$D25</f>
         <v>27.177569999999999</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A19" s="28" t="str">
+      <c r="A19" s="30" t="str">
         <f>Biopax!$A26</f>
         <v>mulGrpAg</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="33">
         <f>Biopax!$C26</f>
         <v>827</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="34">
         <f>Biopax!$D26</f>
         <v>65.769912000000005</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="33">
         <f>Ara!$C26</f>
         <v>753.010989</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="34">
         <f>Ara!$D26</f>
         <v>83.12</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="33">
         <f>Wheat!$C26</f>
         <v>780.01851899999997</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="34">
         <f>Wheat!$D26</f>
         <v>56.32</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A20" s="28" t="str">
+      <c r="A20" s="30" t="str">
         <f>Biopax!$A27</f>
         <v>nestAg</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="33">
         <f>Biopax!$C27</f>
         <v>10.677083</v>
       </c>
-      <c r="C20" s="29">
+      <c r="C20" s="34">
         <f>Biopax!$D27</f>
         <v>22.274509999999999</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="33">
         <f>Ara!$C27</f>
         <v>20.428571000000002</v>
       </c>
-      <c r="E20" s="29">
+      <c r="E20" s="34">
         <f>Ara!$D27</f>
         <v>26.955752</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="33">
         <f>Wheat!$C27</f>
         <v>19.745097999999999</v>
       </c>
-      <c r="G20" s="29">
+      <c r="G20" s="34">
         <f>Wheat!$D27</f>
         <v>24.944444000000001</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A21" s="28" t="str">
+      <c r="A21" s="30" t="str">
         <f>Biopax!$A28</f>
         <v>exist</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="33">
         <f>Biopax!$C28</f>
         <v>31.053763</v>
       </c>
-      <c r="C21" s="29">
+      <c r="C21" s="34">
         <f>Biopax!$D28</f>
         <v>30.904254999999999</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="33">
         <f>Ara!$C28</f>
         <v>21.775281</v>
       </c>
-      <c r="E21" s="29">
+      <c r="E21" s="34">
         <f>Ara!$D28</f>
         <v>36.989691000000001</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="33">
         <f>Wheat!$C28</f>
         <v>19.142856999999999</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="34">
         <f>Wheat!$D28</f>
         <v>34.734693999999998</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A22" s="28" t="str">
+      <c r="A22" s="30" t="str">
         <f>Biopax!$A29</f>
         <v>existAg</v>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="33">
         <f>Biopax!$C29</f>
         <v>59.613208</v>
       </c>
-      <c r="C22" s="29">
+      <c r="C22" s="34">
         <f>Biopax!$D29</f>
         <v>51.344828</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="33">
         <f>Ara!$C29</f>
         <v>25.355768999999999</v>
       </c>
-      <c r="E22" s="29">
+      <c r="E22" s="34">
         <f>Ara!$D29</f>
         <v>62.617283999999998</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="33">
         <f>Wheat!$C29</f>
         <v>36.047618999999997</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="34">
         <f>Wheat!$D29</f>
         <v>59.063063</v>
       </c>

</xml_diff>

<commit_message>
Cleaning. Commenting. Adding figures and explainations. Preparing for the SWAT4LS paper.
</commit_message>
<xml_diff>
--- a/results/gdb_benchmark_results.xlsx
+++ b/results/gdb_benchmark_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandizi/Documents/Work/RRes/events/2018_swat4ls/paper/graphdb-benchmarks/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982F210C-75DF-5D47-AABF-C6DF29966479}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405F3D1C-2322-BA46-AAE1-2E9144F3395D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,9 +493,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -513,6 +510,9 @@
     </xf>
     <xf numFmtId="4" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4896,15 +4896,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -5369,15 +5369,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -5839,15 +5839,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -6292,7 +6292,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6389,8 +6389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CD3143-BDBF-FD41-9A6E-2395CA27F127}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6399,654 +6399,654 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="27" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="30" t="str">
+      <c r="A2" s="29" t="str">
         <f>Biopax!$A9</f>
         <v>cnt</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="32">
         <f>Biopax!$C9</f>
         <v>4.9505E-2</v>
       </c>
-      <c r="C2" s="34">
+      <c r="C2" s="33">
         <f>Biopax!$D9</f>
         <v>622.47959200000003</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D2" s="32">
         <f>Ara!$C9</f>
         <v>0.47169800000000001</v>
       </c>
-      <c r="E2" s="34">
+      <c r="E2" s="33">
         <f>Ara!$D9</f>
         <v>5543.3195880000003</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="32">
         <f>Wheat!$C9</f>
         <v>0.70454499999999998</v>
       </c>
-      <c r="G2" s="34">
+      <c r="G2" s="33">
         <f>Wheat!$D9</f>
         <v>14721.444444000001</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="30" t="str">
+      <c r="A3" s="29" t="str">
         <f>Biopax!$A10</f>
         <v>cntType</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="32">
         <f>Biopax!$C10</f>
         <v>0.76</v>
       </c>
-      <c r="C3" s="34">
+      <c r="C3" s="33">
         <f>Biopax!$D10</f>
         <v>2.548387</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="32">
         <f>Ara!$C10</f>
         <v>5.7818180000000003</v>
       </c>
-      <c r="E3" s="34">
+      <c r="E3" s="33">
         <f>Ara!$D10</f>
         <v>5.0206189999999999</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="32">
         <f>Wheat!$C10</f>
         <v>6.5729170000000003</v>
       </c>
-      <c r="G3" s="34">
+      <c r="G3" s="33">
         <f>Wheat!$D10</f>
         <v>13.847826</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="30" t="str">
+      <c r="A4" s="29" t="str">
         <f>Biopax!$A11</f>
         <v>cntRel</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="32">
         <f>Biopax!$C11</f>
         <v>0.114286</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="33">
         <f>Biopax!$D11</f>
         <v>64.877778000000006</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="32">
         <f>Ara!$C11</f>
         <v>0.36274499999999998</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="33">
         <f>Ara!$D11</f>
         <v>546.69662900000003</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="32">
         <f>Wheat!$C11</f>
         <v>0.655914</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="33">
         <f>Wheat!$D11</f>
         <v>1401.9534880000001</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="30" t="str">
+      <c r="A5" s="29" t="str">
         <f>Biopax!$A12</f>
         <v>cntRelType</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="32">
         <f>Biopax!$C12</f>
         <v>1.6727270000000001</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="33">
         <f>Biopax!$D12</f>
         <v>34.025641</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="32">
         <f>Ara!$C12</f>
         <v>6.8738739999999998</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="33">
         <f>Ara!$D12</f>
         <v>92.782608999999994</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <f>Wheat!$C12</f>
         <v>8</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="33">
         <f>Wheat!$D12</f>
         <v>100.835052</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A6" s="30" t="str">
+      <c r="A6" s="29" t="str">
         <f>Biopax!$A13</f>
         <v>sel</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="32">
         <f>Biopax!$C13</f>
         <v>0.31428600000000001</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="33">
         <f>Biopax!$D13</f>
         <v>6.1818179999999998</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="32">
         <f>Ara!$C13</f>
         <v>0.76087000000000005</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="33">
         <f>Ara!$D13</f>
         <v>4.6306310000000002</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="32">
         <f>Wheat!$C13</f>
         <v>1.605769</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="33">
         <f>Wheat!$D13</f>
         <v>6.9036140000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="30" t="str">
+      <c r="A7" s="29" t="str">
         <f>Biopax!$A14</f>
         <v>join</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="32">
         <f>Biopax!$C14</f>
         <v>1.0659339999999999</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="33">
         <f>Biopax!$D14</f>
         <v>8.6190479999999994</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="32">
         <f>Ara!$C14</f>
         <v>1.448</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="33">
         <f>Ara!$D14</f>
         <v>9.0099009999999993</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="32">
         <f>Wheat!$C14</f>
         <v>1.535088</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="33">
         <f>Wheat!$D14</f>
         <v>9.8627450000000003</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="30" t="str">
+      <c r="A8" s="29" t="str">
         <f>Biopax!$A15</f>
         <v>joinRel</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="32">
         <f>Biopax!$C15</f>
         <v>1.194175</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="33">
         <f>Biopax!$D15</f>
         <v>13.4</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="32">
         <f>Ara!$C15</f>
         <v>1.8658539999999999</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="33">
         <f>Ara!$D15</f>
         <v>17.393162</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <f>Wheat!$C15</f>
         <v>4.68</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="33">
         <f>Wheat!$D15</f>
         <v>21.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="30" t="str">
+      <c r="A9" s="29" t="str">
         <f>Biopax!$A16</f>
         <v>joinFilter</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <f>Biopax!$C16</f>
         <v>3.7083330000000001</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="33">
         <f>Biopax!$D16</f>
         <v>9.5775860000000002</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="32">
         <f>Ara!$C16</f>
         <v>8.7522120000000001</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="33">
         <f>Ara!$D16</f>
         <v>10.4</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <f>Wheat!$C16</f>
         <v>9.4180329999999994</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="33">
         <f>Wheat!$D16</f>
         <v>10.657895</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="30" t="str">
+      <c r="A10" s="29" t="str">
         <f>Biopax!$A17</f>
         <v>joinRe</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="32">
         <f>Biopax!$C17</f>
         <v>3.913043</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="33">
         <f>Biopax!$D17</f>
         <v>10.494624</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="32">
         <f>Ara!$C17</f>
         <v>5.8192769999999996</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="33">
         <f>Ara!$D17</f>
         <v>18.807338999999999</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="32">
         <f>Wheat!$C17</f>
         <v>5.9545450000000004</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="33">
         <f>Wheat!$D17</f>
         <v>10.666667</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="30" t="str">
+      <c r="A11" s="29" t="str">
         <f>Biopax!$A18</f>
         <v>joinReif</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="32">
         <f>Biopax!$C18</f>
         <v>6.8415840000000001</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="33">
         <f>Biopax!$D18</f>
         <v>373.79411800000003</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="32">
         <f>Ara!$C18</f>
         <v>491.942857</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="33">
         <f>Ara!$D18</f>
         <v>60.181818</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="32">
         <f>Wheat!$C18</f>
         <v>14.741935</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="33">
         <f>Wheat!$D18</f>
         <v>66.676190000000005</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A12" s="30" t="str">
+      <c r="A12" s="29" t="str">
         <f>Biopax!$A19</f>
         <v>varPathC</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="32">
         <f>Biopax!$C19</f>
         <v>0.61904800000000004</v>
       </c>
-      <c r="C12" s="34">
+      <c r="C12" s="33">
         <f>Biopax!$D19</f>
         <v>27.914894</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="32">
         <f>Ara!$C19</f>
         <v>1.8921570000000001</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="33">
         <f>Ara!$D19</f>
         <v>25.590909</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="32">
         <f>Wheat!$C19</f>
         <v>1.81</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="33">
         <f>Wheat!$D19</f>
         <v>25.862745</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A13" s="30" t="str">
+      <c r="A13" s="29" t="str">
         <f>Biopax!$A20</f>
         <v>varPath</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="32">
         <f>Biopax!$C20</f>
         <v>5.1397849999999998</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="33">
         <f>Biopax!$D20</f>
         <v>89.483146000000005</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="32">
         <f>Ara!$C20</f>
         <v>7.5833329999999997</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="33">
         <f>Ara!$D20</f>
         <v>18.135922000000001</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="32">
         <f>Wheat!$C20</f>
         <v>4.0416670000000003</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="33">
         <f>Wheat!$D20</f>
         <v>33.349592999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="30" t="str">
+      <c r="A14" s="29" t="str">
         <f>Biopax!$A21</f>
         <v>2union</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="32">
         <f>Biopax!$C21</f>
         <v>11.172043</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="33">
         <f>Biopax!$D21</f>
         <v>12.308510999999999</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D14" s="32">
         <f>Ara!$C21</f>
         <v>10.340206</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="33">
         <f>Ara!$D21</f>
         <v>12.383838000000001</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="32">
         <f>Wheat!$C21</f>
         <v>12.25</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="33">
         <f>Wheat!$D21</f>
         <v>19.73</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="30" t="str">
+      <c r="A15" s="29" t="str">
         <f>Biopax!$A22</f>
         <v>2union1Nest</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B15" s="32">
         <f>Biopax!$C22</f>
         <v>30.958333</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="33">
         <f>Biopax!$D22</f>
         <v>11.049020000000001</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="32">
         <f>Ara!$C22</f>
         <v>44.315789000000002</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="33">
         <f>Ara!$D22</f>
         <v>11.75</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="32">
         <f>Wheat!$C22</f>
         <v>41.304761999999997</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="33">
         <f>Wheat!$D22</f>
         <v>11.644231</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A16" s="30" t="str">
+      <c r="A16" s="29" t="str">
         <f>Biopax!$A23</f>
         <v>pway</v>
       </c>
-      <c r="B16" s="33">
+      <c r="B16" s="32">
         <f>Biopax!$C23</f>
         <v>4.9519229999999999</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="33">
         <f>Biopax!$D23</f>
         <v>38.512605000000001</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="32">
         <f>Ara!$C23</f>
         <v>11.361905</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="33">
         <f>Ara!$D23</f>
         <v>36.090909000000003</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="32">
         <f>Wheat!$C23</f>
         <v>8.3406590000000005</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="33">
         <f>Wheat!$D23</f>
         <v>34.221238999999997</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A17" s="30" t="str">
+      <c r="A17" s="29" t="str">
         <f>Biopax!$A24</f>
         <v>grp</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="32">
         <f>Biopax!$C24</f>
         <v>8.9894739999999995</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="33">
         <f>Biopax!$D24</f>
         <v>21.039216</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="32">
         <f>Ara!$C24</f>
         <v>13.53012</v>
       </c>
-      <c r="E17" s="34">
+      <c r="E17" s="33">
         <f>Ara!$D24</f>
         <v>26.521277000000001</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="32">
         <f>Wheat!$C24</f>
         <v>14.344086000000001</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="33">
         <f>Wheat!$D24</f>
         <v>23.847826000000001</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A18" s="30" t="str">
+      <c r="A18" s="29" t="str">
         <f>Biopax!$A25</f>
         <v>grpAg</v>
       </c>
-      <c r="B18" s="33">
+      <c r="B18" s="32">
         <f>Biopax!$C25</f>
         <v>10.757009</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="33">
         <f>Biopax!$D25</f>
         <v>23.666667</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="32">
         <f>Ara!$C25</f>
         <v>19.221239000000001</v>
       </c>
-      <c r="E18" s="34">
+      <c r="E18" s="33">
         <f>Ara!$D25</f>
         <v>30.169643000000001</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="32">
         <f>Wheat!$C25</f>
         <v>18.600000000000001</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="33">
         <f>Wheat!$D25</f>
         <v>27.177569999999999</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A19" s="30" t="str">
+      <c r="A19" s="29" t="str">
         <f>Biopax!$A26</f>
         <v>mulGrpAg</v>
       </c>
-      <c r="B19" s="33">
+      <c r="B19" s="32">
         <f>Biopax!$C26</f>
         <v>827</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="33">
         <f>Biopax!$D26</f>
         <v>65.769912000000005</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="32">
         <f>Ara!$C26</f>
         <v>753.010989</v>
       </c>
-      <c r="E19" s="34">
+      <c r="E19" s="33">
         <f>Ara!$D26</f>
         <v>83.12</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="32">
         <f>Wheat!$C26</f>
         <v>780.01851899999997</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="33">
         <f>Wheat!$D26</f>
         <v>56.32</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A20" s="30" t="str">
+      <c r="A20" s="29" t="str">
         <f>Biopax!$A27</f>
         <v>nestAg</v>
       </c>
-      <c r="B20" s="33">
+      <c r="B20" s="32">
         <f>Biopax!$C27</f>
         <v>10.677083</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="33">
         <f>Biopax!$D27</f>
         <v>22.274509999999999</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="32">
         <f>Ara!$C27</f>
         <v>20.428571000000002</v>
       </c>
-      <c r="E20" s="34">
+      <c r="E20" s="33">
         <f>Ara!$D27</f>
         <v>26.955752</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="32">
         <f>Wheat!$C27</f>
         <v>19.745097999999999</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="33">
         <f>Wheat!$D27</f>
         <v>24.944444000000001</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A21" s="30" t="str">
+      <c r="A21" s="29" t="str">
         <f>Biopax!$A28</f>
         <v>exist</v>
       </c>
-      <c r="B21" s="33">
+      <c r="B21" s="32">
         <f>Biopax!$C28</f>
         <v>31.053763</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="33">
         <f>Biopax!$D28</f>
         <v>30.904254999999999</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="32">
         <f>Ara!$C28</f>
         <v>21.775281</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="33">
         <f>Ara!$D28</f>
         <v>36.989691000000001</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="32">
         <f>Wheat!$C28</f>
         <v>19.142856999999999</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="33">
         <f>Wheat!$D28</f>
         <v>34.734693999999998</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A22" s="30" t="str">
+      <c r="A22" s="29" t="str">
         <f>Biopax!$A29</f>
         <v>existAg</v>
       </c>
-      <c r="B22" s="33">
+      <c r="B22" s="32">
         <f>Biopax!$C29</f>
         <v>59.613208</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="33">
         <f>Biopax!$D29</f>
         <v>51.344828</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="32">
         <f>Ara!$C29</f>
         <v>25.355768999999999</v>
       </c>
-      <c r="E22" s="34">
+      <c r="E22" s="33">
         <f>Ara!$D29</f>
         <v>62.617283999999998</v>
       </c>
-      <c r="F22" s="33">
+      <c r="F22" s="32">
         <f>Wheat!$C29</f>
         <v>36.047618999999997</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="33">
         <f>Wheat!$D29</f>
         <v>59.063063</v>
       </c>

</xml_diff>

<commit_message>
2x2 version of the query performance charts.
</commit_message>
<xml_diff>
--- a/results/gdb_benchmark_results.xlsx
+++ b/results/gdb_benchmark_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandizi/Documents/Work/RRes/events/2018_swat4ls/paper/graphdb-benchmarks/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405F3D1C-2322-BA46-AAE1-2E9144F3395D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29955939-EB7A-104E-8666-BFADCB3ABFF5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,14 +19,10 @@
     <sheet name="Load Chart" sheetId="5" r:id="rId4"/>
     <sheet name="Performance Chart" sheetId="6" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Performance Chart'!$A$60:$L$103</definedName>
+  </definedNames>
   <calcPr calcId="179021"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1312,7 +1308,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Performance Chart'!$B$1</c:f>
+              <c:f>'Performance Chart'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1343,7 +1339,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Performance Chart'!$A$2:$A$22</c:f>
+              <c:f>'Performance Chart'!$A$3:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -1414,7 +1410,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Performance Chart'!$B$2:$B$22</c:f>
+              <c:f>'Performance Chart'!$B$3:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1495,7 +1491,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Performance Chart'!$C$1</c:f>
+              <c:f>'Performance Chart'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1526,7 +1522,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Performance Chart'!$A$2:$A$22</c:f>
+              <c:f>'Performance Chart'!$A$3:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -1597,7 +1593,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Performance Chart'!$C$2:$C$22</c:f>
+              <c:f>'Performance Chart'!$C$3:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1678,7 +1674,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Performance Chart'!$D$1</c:f>
+              <c:f>'Performance Chart'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1709,7 +1705,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Performance Chart'!$A$2:$A$22</c:f>
+              <c:f>'Performance Chart'!$A$3:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -1780,7 +1776,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Performance Chart'!$D$2:$D$22</c:f>
+              <c:f>'Performance Chart'!$D$3:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1861,7 +1857,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Performance Chart'!$E$1</c:f>
+              <c:f>'Performance Chart'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1892,7 +1888,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Performance Chart'!$A$2:$A$22</c:f>
+              <c:f>'Performance Chart'!$A$3:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -1963,7 +1959,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Performance Chart'!$E$2:$E$22</c:f>
+              <c:f>'Performance Chart'!$E$3:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2044,7 +2040,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Performance Chart'!$F$1</c:f>
+              <c:f>'Performance Chart'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2075,7 +2071,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Performance Chart'!$A$2:$A$22</c:f>
+              <c:f>'Performance Chart'!$A$3:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -2146,7 +2142,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Performance Chart'!$F$2:$F$22</c:f>
+              <c:f>'Performance Chart'!$F$3:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2227,7 +2223,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Performance Chart'!$G$1</c:f>
+              <c:f>'Performance Chart'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2258,7 +2254,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Performance Chart'!$A$2:$A$22</c:f>
+              <c:f>'Performance Chart'!$A$3:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -2329,7 +2325,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Performance Chart'!$G$2:$G$22</c:f>
+              <c:f>'Performance Chart'!$G$3:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2425,6 +2421,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" cap="none" baseline="0"/>
+                  <a:t>Execution times (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2627,6 +2678,1818 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Chart'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>neo4j/bpax</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkUpDiag">
+              <a:fgClr>
+                <a:srgbClr val="0432FF"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="0432FF"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance Chart'!$A$3:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>cnt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cntType</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>cntRel</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cntRelType</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sel</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>join</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>joinRel</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>joinFilter</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>joinRe</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>joinReif</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>varPathC</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>varPath</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2union</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2union1Nest</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>pway</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>grp</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>grpAg</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>mulGrpAg</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>nestAg</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>exist</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>existAg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance Chart'!$B$3:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>4.9505E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.114286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6727270000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.31428600000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0659339999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.194175</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.7083330000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.913043</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.8415840000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.61904800000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.1397849999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.172043</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30.958333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.9519229999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.9894739999999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.757009</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>827</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.677083</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>31.053763</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>59.613208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2F7A-A143-B09E-676C69EEC8E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Chart'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>virt/bpax</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkDnDiag">
+              <a:fgClr>
+                <a:srgbClr val="FF0000"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance Chart'!$A$3:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>cnt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cntType</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>cntRel</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cntRelType</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sel</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>join</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>joinRel</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>joinFilter</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>joinRe</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>joinReif</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>varPathC</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>varPath</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2union</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2union1Nest</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>pway</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>grp</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>grpAg</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>mulGrpAg</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>nestAg</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>exist</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>existAg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance Chart'!$C$3:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>622.47959200000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.548387</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.877778000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.025641</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1818179999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6190479999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.5775860000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.494624</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>373.79411800000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27.914894</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>89.483146000000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.308510999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.049020000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38.512605000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21.039216</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23.666667</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>65.769912000000005</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22.274509999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30.904254999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>51.344828</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2F7A-A143-B09E-676C69EEC8E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="199"/>
+        <c:axId val="966579936"/>
+        <c:axId val="972506032"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="966579936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="972506032"/>
+        <c:crossesAt val="1"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="972506032"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="50000"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg2"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="966579936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Chart'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>neo4j/ara</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkUpDiag">
+              <a:fgClr>
+                <a:srgbClr val="0432FF"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="0432FF"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance Chart'!$A$3:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>cnt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cntType</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>cntRel</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cntRelType</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sel</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>join</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>joinRel</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>joinFilter</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>joinRe</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>joinReif</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>varPathC</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>varPath</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2union</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2union1Nest</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>pway</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>grp</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>grpAg</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>mulGrpAg</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>nestAg</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>exist</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>existAg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance Chart'!$D$3:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.47169800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7818180000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.36274499999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8738739999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.76087000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.448</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8658539999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.7522120000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.8192769999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>491.942857</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8921570000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.5833329999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.340206</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44.315789000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.361905</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.53012</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.221239000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>753.010989</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20.428571000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21.775281</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25.355768999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F234-744B-9CE4-0C7D974067B0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Chart'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>virt/ara</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkDnDiag">
+              <a:fgClr>
+                <a:srgbClr val="FF0000"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance Chart'!$A$3:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>cnt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cntType</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>cntRel</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cntRelType</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sel</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>join</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>joinRel</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>joinFilter</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>joinRe</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>joinReif</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>varPathC</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>varPath</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2union</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2union1Nest</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>pway</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>grp</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>grpAg</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>mulGrpAg</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>nestAg</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>exist</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>existAg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance Chart'!$E$3:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>5543.3195880000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0206189999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>546.69662900000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92.782608999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.6306310000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0099009999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.393162</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.807338999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60.181818</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.590909</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18.135922000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.383838000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36.090909000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26.521277000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30.169643000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>83.12</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26.955752</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>36.989691000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>62.617283999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F234-744B-9CE4-0C7D974067B0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="199"/>
+        <c:axId val="966579936"/>
+        <c:axId val="972506032"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="966579936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="972506032"/>
+        <c:crossesAt val="1"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="972506032"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="50000"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg2"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="966579936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Chart'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>neo4j/wheat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkUpDiag">
+              <a:fgClr>
+                <a:srgbClr val="0432FF"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="0432FF"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance Chart'!$A$3:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>cnt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cntType</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>cntRel</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cntRelType</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sel</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>join</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>joinRel</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>joinFilter</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>joinRe</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>joinReif</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>varPathC</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>varPath</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2union</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2union1Nest</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>pway</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>grp</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>grpAg</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>mulGrpAg</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>nestAg</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>exist</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>existAg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance Chart'!$F$3:$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.70454499999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5729170000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.655914</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.605769</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.535088</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.4180329999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.9545450000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.741935</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0416670000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41.304761999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.3406590000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14.344086000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>780.01851899999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.745097999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.142856999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>36.047618999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E6FF-D646-BB5B-E45B23DCE817}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Chart'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>virt/wheat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkDnDiag">
+              <a:fgClr>
+                <a:srgbClr val="FF0000"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance Chart'!$A$3:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>cnt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cntType</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>cntRel</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cntRelType</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sel</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>join</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>joinRel</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>joinFilter</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>joinRe</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>joinReif</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>varPathC</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>varPath</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2union</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2union1Nest</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>pway</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>grp</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>grpAg</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>mulGrpAg</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>nestAg</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>exist</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>existAg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance Chart'!$G$3:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>14721.444444000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.847826</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1401.9534880000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100.835052</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9036140000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8627450000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.657895</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.666667</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66.676190000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.862745</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.349592999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19.73</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.644231</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>34.221238999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23.847826000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27.177569999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>56.32</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24.944444000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>34.734693999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>59.063063</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E6FF-D646-BB5B-E45B23DCE817}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="199"/>
+        <c:axId val="966579936"/>
+        <c:axId val="972506032"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="966579936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="972506032"/>
+        <c:crossesAt val="1"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="972506032"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="50000"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg2"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="966579936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2707,6 +4570,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3224,6 +5207,1506 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="212">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="212">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="212">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="212">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3770,13 +7253,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>122827</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>249382</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>63499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3797,6 +7280,120 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>392466</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>33473</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>570265</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>151868</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EAB3BFB-B8F9-AD4B-8D54-9DF9105FE0BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>72103</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>25398</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A20ACFD6-5091-0345-8B7C-52E146327A56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>391584</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>73161</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>569383</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>26456</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B06CF755-4D78-8F4D-98C3-83D9BBA44917}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6387,10 +9984,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CD3143-BDBF-FD41-9A6E-2395CA27F127}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6398,666 +9995,668 @@
     <col min="1" max="7" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="27" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+    <row r="2" spans="1:7" s="27" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D2" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E2" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G2" s="31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="29" t="str">
+    <row r="3" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" s="29" t="str">
         <f>Biopax!$A9</f>
         <v>cnt</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B3" s="32">
         <f>Biopax!$C9</f>
         <v>4.9505E-2</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C3" s="33">
         <f>Biopax!$D9</f>
         <v>622.47959200000003</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D3" s="32">
         <f>Ara!$C9</f>
         <v>0.47169800000000001</v>
       </c>
-      <c r="E2" s="33">
+      <c r="E3" s="33">
         <f>Ara!$D9</f>
         <v>5543.3195880000003</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F3" s="32">
         <f>Wheat!$C9</f>
         <v>0.70454499999999998</v>
       </c>
-      <c r="G2" s="33">
+      <c r="G3" s="33">
         <f>Wheat!$D9</f>
         <v>14721.444444000001</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="29" t="str">
+    <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A4" s="29" t="str">
         <f>Biopax!$A10</f>
         <v>cntType</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B4" s="32">
         <f>Biopax!$C10</f>
         <v>0.76</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C4" s="33">
         <f>Biopax!$D10</f>
         <v>2.548387</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D4" s="32">
         <f>Ara!$C10</f>
         <v>5.7818180000000003</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E4" s="33">
         <f>Ara!$D10</f>
         <v>5.0206189999999999</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F4" s="32">
         <f>Wheat!$C10</f>
         <v>6.5729170000000003</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G4" s="33">
         <f>Wheat!$D10</f>
         <v>13.847826</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="29" t="str">
+    <row r="5" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="29" t="str">
         <f>Biopax!$A11</f>
         <v>cntRel</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B5" s="32">
         <f>Biopax!$C11</f>
         <v>0.114286</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C5" s="33">
         <f>Biopax!$D11</f>
         <v>64.877778000000006</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D5" s="32">
         <f>Ara!$C11</f>
         <v>0.36274499999999998</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E5" s="33">
         <f>Ara!$D11</f>
         <v>546.69662900000003</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F5" s="32">
         <f>Wheat!$C11</f>
         <v>0.655914</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G5" s="33">
         <f>Wheat!$D11</f>
         <v>1401.9534880000001</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="29" t="str">
+    <row r="6" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="29" t="str">
         <f>Biopax!$A12</f>
         <v>cntRelType</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B6" s="32">
         <f>Biopax!$C12</f>
         <v>1.6727270000000001</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C6" s="33">
         <f>Biopax!$D12</f>
         <v>34.025641</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D6" s="32">
         <f>Ara!$C12</f>
         <v>6.8738739999999998</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E6" s="33">
         <f>Ara!$D12</f>
         <v>92.782608999999994</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F6" s="32">
         <f>Wheat!$C12</f>
         <v>8</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G6" s="33">
         <f>Wheat!$D12</f>
         <v>100.835052</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A6" s="29" t="str">
+    <row r="7" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="29" t="str">
         <f>Biopax!$A13</f>
         <v>sel</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B7" s="32">
         <f>Biopax!$C13</f>
         <v>0.31428600000000001</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C7" s="33">
         <f>Biopax!$D13</f>
         <v>6.1818179999999998</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D7" s="32">
         <f>Ara!$C13</f>
         <v>0.76087000000000005</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E7" s="33">
         <f>Ara!$D13</f>
         <v>4.6306310000000002</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F7" s="32">
         <f>Wheat!$C13</f>
         <v>1.605769</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G7" s="33">
         <f>Wheat!$D13</f>
         <v>6.9036140000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="29" t="str">
+    <row r="8" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A8" s="29" t="str">
         <f>Biopax!$A14</f>
         <v>join</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B8" s="32">
         <f>Biopax!$C14</f>
         <v>1.0659339999999999</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C8" s="33">
         <f>Biopax!$D14</f>
         <v>8.6190479999999994</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D8" s="32">
         <f>Ara!$C14</f>
         <v>1.448</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E8" s="33">
         <f>Ara!$D14</f>
         <v>9.0099009999999993</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F8" s="32">
         <f>Wheat!$C14</f>
         <v>1.535088</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G8" s="33">
         <f>Wheat!$D14</f>
         <v>9.8627450000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="29" t="str">
+    <row r="9" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="29" t="str">
         <f>Biopax!$A15</f>
         <v>joinRel</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B9" s="32">
         <f>Biopax!$C15</f>
         <v>1.194175</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C9" s="33">
         <f>Biopax!$D15</f>
         <v>13.4</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D9" s="32">
         <f>Ara!$C15</f>
         <v>1.8658539999999999</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E9" s="33">
         <f>Ara!$D15</f>
         <v>17.393162</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F9" s="32">
         <f>Wheat!$C15</f>
         <v>4.68</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G9" s="33">
         <f>Wheat!$D15</f>
         <v>21.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="29" t="str">
+    <row r="10" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="29" t="str">
         <f>Biopax!$A16</f>
         <v>joinFilter</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B10" s="32">
         <f>Biopax!$C16</f>
         <v>3.7083330000000001</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C10" s="33">
         <f>Biopax!$D16</f>
         <v>9.5775860000000002</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D10" s="32">
         <f>Ara!$C16</f>
         <v>8.7522120000000001</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E10" s="33">
         <f>Ara!$D16</f>
         <v>10.4</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F10" s="32">
         <f>Wheat!$C16</f>
         <v>9.4180329999999994</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G10" s="33">
         <f>Wheat!$D16</f>
         <v>10.657895</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="29" t="str">
+    <row r="11" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="29" t="str">
         <f>Biopax!$A17</f>
         <v>joinRe</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B11" s="32">
         <f>Biopax!$C17</f>
         <v>3.913043</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C11" s="33">
         <f>Biopax!$D17</f>
         <v>10.494624</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D11" s="32">
         <f>Ara!$C17</f>
         <v>5.8192769999999996</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E11" s="33">
         <f>Ara!$D17</f>
         <v>18.807338999999999</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F11" s="32">
         <f>Wheat!$C17</f>
         <v>5.9545450000000004</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G11" s="33">
         <f>Wheat!$D17</f>
         <v>10.666667</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="29" t="str">
+    <row r="12" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" s="29" t="str">
         <f>Biopax!$A18</f>
         <v>joinReif</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B12" s="32">
         <f>Biopax!$C18</f>
         <v>6.8415840000000001</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C12" s="33">
         <f>Biopax!$D18</f>
         <v>373.79411800000003</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D12" s="32">
         <f>Ara!$C18</f>
         <v>491.942857</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E12" s="33">
         <f>Ara!$D18</f>
         <v>60.181818</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F12" s="32">
         <f>Wheat!$C18</f>
         <v>14.741935</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G12" s="33">
         <f>Wheat!$D18</f>
         <v>66.676190000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A12" s="29" t="str">
+    <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" s="29" t="str">
         <f>Biopax!$A19</f>
         <v>varPathC</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B13" s="32">
         <f>Biopax!$C19</f>
         <v>0.61904800000000004</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C13" s="33">
         <f>Biopax!$D19</f>
         <v>27.914894</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D13" s="32">
         <f>Ara!$C19</f>
         <v>1.8921570000000001</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E13" s="33">
         <f>Ara!$D19</f>
         <v>25.590909</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F13" s="32">
         <f>Wheat!$C19</f>
         <v>1.81</v>
       </c>
-      <c r="G12" s="33">
+      <c r="G13" s="33">
         <f>Wheat!$D19</f>
         <v>25.862745</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A13" s="29" t="str">
+    <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A14" s="29" t="str">
         <f>Biopax!$A20</f>
         <v>varPath</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B14" s="32">
         <f>Biopax!$C20</f>
         <v>5.1397849999999998</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C14" s="33">
         <f>Biopax!$D20</f>
         <v>89.483146000000005</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D14" s="32">
         <f>Ara!$C20</f>
         <v>7.5833329999999997</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E14" s="33">
         <f>Ara!$D20</f>
         <v>18.135922000000001</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F14" s="32">
         <f>Wheat!$C20</f>
         <v>4.0416670000000003</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G14" s="33">
         <f>Wheat!$D20</f>
         <v>33.349592999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="29" t="str">
+    <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A15" s="29" t="str">
         <f>Biopax!$A21</f>
         <v>2union</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B15" s="32">
         <f>Biopax!$C21</f>
         <v>11.172043</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C15" s="33">
         <f>Biopax!$D21</f>
         <v>12.308510999999999</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D15" s="32">
         <f>Ara!$C21</f>
         <v>10.340206</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E15" s="33">
         <f>Ara!$D21</f>
         <v>12.383838000000001</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F15" s="32">
         <f>Wheat!$C21</f>
         <v>12.25</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G15" s="33">
         <f>Wheat!$D21</f>
         <v>19.73</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="29" t="str">
+    <row r="16" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" s="29" t="str">
         <f>Biopax!$A22</f>
         <v>2union1Nest</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B16" s="32">
         <f>Biopax!$C22</f>
         <v>30.958333</v>
       </c>
-      <c r="C15" s="33">
+      <c r="C16" s="33">
         <f>Biopax!$D22</f>
         <v>11.049020000000001</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D16" s="32">
         <f>Ara!$C22</f>
         <v>44.315789000000002</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E16" s="33">
         <f>Ara!$D22</f>
         <v>11.75</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F16" s="32">
         <f>Wheat!$C22</f>
         <v>41.304761999999997</v>
       </c>
-      <c r="G15" s="33">
+      <c r="G16" s="33">
         <f>Wheat!$D22</f>
         <v>11.644231</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A16" s="29" t="str">
+    <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A17" s="29" t="str">
         <f>Biopax!$A23</f>
         <v>pway</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B17" s="32">
         <f>Biopax!$C23</f>
         <v>4.9519229999999999</v>
       </c>
-      <c r="C16" s="33">
+      <c r="C17" s="33">
         <f>Biopax!$D23</f>
         <v>38.512605000000001</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D17" s="32">
         <f>Ara!$C23</f>
         <v>11.361905</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E17" s="33">
         <f>Ara!$D23</f>
         <v>36.090909000000003</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F17" s="32">
         <f>Wheat!$C23</f>
         <v>8.3406590000000005</v>
       </c>
-      <c r="G16" s="33">
+      <c r="G17" s="33">
         <f>Wheat!$D23</f>
         <v>34.221238999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A17" s="29" t="str">
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A18" s="29" t="str">
         <f>Biopax!$A24</f>
         <v>grp</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B18" s="32">
         <f>Biopax!$C24</f>
         <v>8.9894739999999995</v>
       </c>
-      <c r="C17" s="33">
+      <c r="C18" s="33">
         <f>Biopax!$D24</f>
         <v>21.039216</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D18" s="32">
         <f>Ara!$C24</f>
         <v>13.53012</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E18" s="33">
         <f>Ara!$D24</f>
         <v>26.521277000000001</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F18" s="32">
         <f>Wheat!$C24</f>
         <v>14.344086000000001</v>
       </c>
-      <c r="G17" s="33">
+      <c r="G18" s="33">
         <f>Wheat!$D24</f>
         <v>23.847826000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A18" s="29" t="str">
+    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A19" s="29" t="str">
         <f>Biopax!$A25</f>
         <v>grpAg</v>
       </c>
-      <c r="B18" s="32">
+      <c r="B19" s="32">
         <f>Biopax!$C25</f>
         <v>10.757009</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C19" s="33">
         <f>Biopax!$D25</f>
         <v>23.666667</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D19" s="32">
         <f>Ara!$C25</f>
         <v>19.221239000000001</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E19" s="33">
         <f>Ara!$D25</f>
         <v>30.169643000000001</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F19" s="32">
         <f>Wheat!$C25</f>
         <v>18.600000000000001</v>
       </c>
-      <c r="G18" s="33">
+      <c r="G19" s="33">
         <f>Wheat!$D25</f>
         <v>27.177569999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A19" s="29" t="str">
+    <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A20" s="29" t="str">
         <f>Biopax!$A26</f>
         <v>mulGrpAg</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B20" s="32">
         <f>Biopax!$C26</f>
         <v>827</v>
       </c>
-      <c r="C19" s="33">
+      <c r="C20" s="33">
         <f>Biopax!$D26</f>
         <v>65.769912000000005</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D20" s="32">
         <f>Ara!$C26</f>
         <v>753.010989</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E20" s="33">
         <f>Ara!$D26</f>
         <v>83.12</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F20" s="32">
         <f>Wheat!$C26</f>
         <v>780.01851899999997</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G20" s="33">
         <f>Wheat!$D26</f>
         <v>56.32</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A20" s="29" t="str">
+    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A21" s="29" t="str">
         <f>Biopax!$A27</f>
         <v>nestAg</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B21" s="32">
         <f>Biopax!$C27</f>
         <v>10.677083</v>
       </c>
-      <c r="C20" s="33">
+      <c r="C21" s="33">
         <f>Biopax!$D27</f>
         <v>22.274509999999999</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D21" s="32">
         <f>Ara!$C27</f>
         <v>20.428571000000002</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E21" s="33">
         <f>Ara!$D27</f>
         <v>26.955752</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F21" s="32">
         <f>Wheat!$C27</f>
         <v>19.745097999999999</v>
       </c>
-      <c r="G20" s="33">
+      <c r="G21" s="33">
         <f>Wheat!$D27</f>
         <v>24.944444000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A21" s="29" t="str">
+    <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A22" s="29" t="str">
         <f>Biopax!$A28</f>
         <v>exist</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B22" s="32">
         <f>Biopax!$C28</f>
         <v>31.053763</v>
       </c>
-      <c r="C21" s="33">
+      <c r="C22" s="33">
         <f>Biopax!$D28</f>
         <v>30.904254999999999</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D22" s="32">
         <f>Ara!$C28</f>
         <v>21.775281</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E22" s="33">
         <f>Ara!$D28</f>
         <v>36.989691000000001</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F22" s="32">
         <f>Wheat!$C28</f>
         <v>19.142856999999999</v>
       </c>
-      <c r="G21" s="33">
+      <c r="G22" s="33">
         <f>Wheat!$D28</f>
         <v>34.734693999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A22" s="29" t="str">
+    <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A23" s="29" t="str">
         <f>Biopax!$A29</f>
         <v>existAg</v>
       </c>
-      <c r="B22" s="32">
+      <c r="B23" s="32">
         <f>Biopax!$C29</f>
         <v>59.613208</v>
       </c>
-      <c r="C22" s="33">
+      <c r="C23" s="33">
         <f>Biopax!$D29</f>
         <v>51.344828</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D23" s="32">
         <f>Ara!$C29</f>
         <v>25.355768999999999</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E23" s="33">
         <f>Ara!$D29</f>
         <v>62.617283999999998</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F23" s="32">
         <f>Wheat!$C29</f>
         <v>36.047618999999997</v>
       </c>
-      <c r="G22" s="33">
+      <c r="G23" s="33">
         <f>Wheat!$D29</f>
         <v>59.063063</v>
       </c>
     </row>
-    <row r="50" spans="3:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="C50" s="26" t="s">
+    <row r="51" spans="3:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="C51" s="26" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Back to the vertical layout for the query performance chart.
</commit_message>
<xml_diff>
--- a/results/gdb_benchmark_results.xlsx
+++ b/results/gdb_benchmark_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandizi/Documents/Work/RRes/events/2018_swat4ls/paper/graphdb-benchmarks/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandizi/Documents/Work/RRes/events/2018_swat4ls/paper/Review 1/material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29955939-EB7A-104E-8666-BFADCB3ABFF5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9D28C7-A3A9-CC42-ABA7-9EDD5C9D33C1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Performance Chart" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'Performance Chart'!$A$60:$L$103</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Performance Chart'!$A$52:$J$107</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
 </workbook>
@@ -192,7 +192,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -3167,7 +3167,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3771,7 +3771,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4375,7 +4375,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7287,16 +7287,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>392466</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>33473</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>136072</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>5562</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>570265</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>151868</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>423333</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>125604</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7326,15 +7326,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>152401</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>72103</xdr:rowOff>
+      <xdr:colOff>138754</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>147665</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>25398</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>420289</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>106952</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7363,16 +7363,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>391584</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>73161</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>136136</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>128556</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>569383</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>26456</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>420288</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>88862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8486,13 +8486,13 @@
       <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23.33203125" style="1" customWidth="1"/>
     <col min="2" max="256" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -8503,7 +8503,7 @@
       <c r="F1" s="34"/>
       <c r="G1" s="34"/>
     </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="20.25" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -8520,7 +8520,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="20.25" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -8536,7 +8536,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -8549,7 +8549,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
@@ -8567,7 +8567,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -8583,7 +8583,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -8597,7 +8597,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
@@ -8613,7 +8613,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
@@ -8630,7 +8630,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
@@ -8645,7 +8645,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
@@ -8660,7 +8660,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
@@ -8675,7 +8675,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
@@ -8690,7 +8690,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
@@ -8705,7 +8705,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="8" t="s">
         <v>21</v>
       </c>
@@ -8720,7 +8720,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>22</v>
       </c>
@@ -8735,7 +8735,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="20" customHeight="1">
       <c r="A17" s="8" t="s">
         <v>23</v>
       </c>
@@ -8750,7 +8750,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="20" customHeight="1">
       <c r="A18" s="8" t="s">
         <v>24</v>
       </c>
@@ -8765,7 +8765,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="20" customHeight="1">
       <c r="A19" s="8" t="s">
         <v>25</v>
       </c>
@@ -8780,7 +8780,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="20" customHeight="1">
       <c r="A20" s="8" t="s">
         <v>26</v>
       </c>
@@ -8795,7 +8795,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="20" customHeight="1">
       <c r="A21" s="8" t="s">
         <v>27</v>
       </c>
@@ -8810,7 +8810,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="20" customHeight="1">
       <c r="A22" s="8" t="s">
         <v>28</v>
       </c>
@@ -8825,7 +8825,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="20" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>29</v>
       </c>
@@ -8840,7 +8840,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="20" customHeight="1">
       <c r="A24" s="8" t="s">
         <v>30</v>
       </c>
@@ -8855,7 +8855,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="20" customHeight="1">
       <c r="A25" s="8" t="s">
         <v>31</v>
       </c>
@@ -8870,7 +8870,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="20" customHeight="1">
       <c r="A26" s="8" t="s">
         <v>32</v>
       </c>
@@ -8885,7 +8885,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="20" customHeight="1">
       <c r="A27" s="8" t="s">
         <v>33</v>
       </c>
@@ -8900,7 +8900,7 @@
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="20" customHeight="1">
       <c r="A28" s="8" t="s">
         <v>34</v>
       </c>
@@ -8915,7 +8915,7 @@
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="20" customHeight="1">
       <c r="A29" s="8" t="s">
         <v>35</v>
       </c>
@@ -8956,7 +8956,7 @@
       <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21.83203125" style="19" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="19" customWidth="1"/>
@@ -8965,7 +8965,7 @@
     <col min="5" max="256" width="16.33203125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -8976,7 +8976,7 @@
       <c r="F1" s="34"/>
       <c r="G1" s="34"/>
     </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="20.25" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -8993,7 +8993,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="20.25" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -9008,7 +9008,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -9021,7 +9021,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
@@ -9039,7 +9039,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -9054,7 +9054,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -9067,7 +9067,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
@@ -9084,7 +9084,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
@@ -9101,7 +9101,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
@@ -9116,7 +9116,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
@@ -9131,7 +9131,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
@@ -9146,7 +9146,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
@@ -9161,7 +9161,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
@@ -9176,7 +9176,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="8" t="s">
         <v>21</v>
       </c>
@@ -9191,7 +9191,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>22</v>
       </c>
@@ -9206,7 +9206,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="16"/>
     </row>
-    <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="20" customHeight="1">
       <c r="A17" s="8" t="s">
         <v>23</v>
       </c>
@@ -9221,7 +9221,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="20" customHeight="1">
       <c r="A18" s="8" t="s">
         <v>24</v>
       </c>
@@ -9236,7 +9236,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="20" customHeight="1">
       <c r="A19" s="8" t="s">
         <v>25</v>
       </c>
@@ -9251,7 +9251,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="20" customHeight="1">
       <c r="A20" s="8" t="s">
         <v>26</v>
       </c>
@@ -9266,7 +9266,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="20" customHeight="1">
       <c r="A21" s="8" t="s">
         <v>27</v>
       </c>
@@ -9281,7 +9281,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="20" customHeight="1">
       <c r="A22" s="8" t="s">
         <v>28</v>
       </c>
@@ -9296,7 +9296,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="20" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>29</v>
       </c>
@@ -9311,7 +9311,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="20" customHeight="1">
       <c r="A24" s="8" t="s">
         <v>30</v>
       </c>
@@ -9326,7 +9326,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="20" customHeight="1">
       <c r="A25" s="8" t="s">
         <v>31</v>
       </c>
@@ -9341,7 +9341,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="20" customHeight="1">
       <c r="A26" s="8" t="s">
         <v>32</v>
       </c>
@@ -9356,7 +9356,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="15"/>
     </row>
-    <row r="27" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="20" customHeight="1">
       <c r="A27" s="8" t="s">
         <v>33</v>
       </c>
@@ -9371,7 +9371,7 @@
       <c r="F27" s="10"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="20" customHeight="1">
       <c r="A28" s="8" t="s">
         <v>34</v>
       </c>
@@ -9386,7 +9386,7 @@
       <c r="F28" s="10"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="20" customHeight="1">
       <c r="A29" s="8" t="s">
         <v>35</v>
       </c>
@@ -9427,7 +9427,7 @@
       <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21" style="21" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="21" customWidth="1"/>
@@ -9435,7 +9435,7 @@
     <col min="4" max="256" width="16.33203125" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -9446,7 +9446,7 @@
       <c r="F1" s="34"/>
       <c r="G1" s="34"/>
     </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="20.25" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -9463,7 +9463,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="20.25" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -9479,7 +9479,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -9492,7 +9492,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
@@ -9510,7 +9510,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -9525,7 +9525,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -9538,7 +9538,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
@@ -9555,7 +9555,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
@@ -9572,7 +9572,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
@@ -9587,7 +9587,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
@@ -9602,7 +9602,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
@@ -9617,7 +9617,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
@@ -9632,7 +9632,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
@@ -9647,7 +9647,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="8" t="s">
         <v>21</v>
       </c>
@@ -9662,7 +9662,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>22</v>
       </c>
@@ -9677,7 +9677,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="20" customHeight="1">
       <c r="A17" s="8" t="s">
         <v>23</v>
       </c>
@@ -9692,7 +9692,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="20" customHeight="1">
       <c r="A18" s="8" t="s">
         <v>24</v>
       </c>
@@ -9707,7 +9707,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="20" customHeight="1">
       <c r="A19" s="8" t="s">
         <v>25</v>
       </c>
@@ -9722,7 +9722,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="20" customHeight="1">
       <c r="A20" s="8" t="s">
         <v>26</v>
       </c>
@@ -9737,7 +9737,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="20" customHeight="1">
       <c r="A21" s="8" t="s">
         <v>27</v>
       </c>
@@ -9752,7 +9752,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="20" customHeight="1">
       <c r="A22" s="8" t="s">
         <v>28</v>
       </c>
@@ -9767,7 +9767,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="20" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>29</v>
       </c>
@@ -9782,7 +9782,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="20" customHeight="1">
       <c r="A24" s="8" t="s">
         <v>30</v>
       </c>
@@ -9797,7 +9797,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="20" customHeight="1">
       <c r="A25" s="8" t="s">
         <v>31</v>
       </c>
@@ -9812,7 +9812,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="20" customHeight="1">
       <c r="A26" s="8" t="s">
         <v>32</v>
       </c>
@@ -9827,7 +9827,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="20" customHeight="1">
       <c r="A27" s="8" t="s">
         <v>33</v>
       </c>
@@ -9842,7 +9842,7 @@
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="20" customHeight="1">
       <c r="A28" s="8" t="s">
         <v>34</v>
       </c>
@@ -9857,7 +9857,7 @@
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="20" customHeight="1">
       <c r="A29" s="8" t="s">
         <v>35</v>
       </c>
@@ -9892,7 +9892,7 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="2" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
@@ -9900,7 +9900,7 @@
     <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="25" customFormat="1" ht="14">
       <c r="A1" s="25" t="s">
         <v>36</v>
       </c>
@@ -9914,7 +9914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="14">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -9931,7 +9931,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="14">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -9948,7 +9948,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="14">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -9965,12 +9965,12 @@
         <v>8.3211833333333338</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="14">
       <c r="E8" s="26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="13" customHeight="1">
       <c r="E9" s="26" t="s">
         <v>49</v>
       </c>
@@ -9986,16 +9986,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CD3143-BDBF-FD41-9A6E-2395CA27F127}">
   <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q69" sqref="Q69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="7" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" s="27" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" s="27" customFormat="1" ht="14">
       <c r="A2" s="28" t="s">
         <v>40</v>
       </c>
@@ -10018,7 +10018,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="14">
       <c r="A3" s="29" t="str">
         <f>Biopax!$A9</f>
         <v>cnt</v>
@@ -10048,7 +10048,7 @@
         <v>14721.444444000001</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="14">
       <c r="A4" s="29" t="str">
         <f>Biopax!$A10</f>
         <v>cntType</v>
@@ -10078,7 +10078,7 @@
         <v>13.847826</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="14">
       <c r="A5" s="29" t="str">
         <f>Biopax!$A11</f>
         <v>cntRel</v>
@@ -10108,7 +10108,7 @@
         <v>1401.9534880000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="14">
       <c r="A6" s="29" t="str">
         <f>Biopax!$A12</f>
         <v>cntRelType</v>
@@ -10138,7 +10138,7 @@
         <v>100.835052</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="14">
       <c r="A7" s="29" t="str">
         <f>Biopax!$A13</f>
         <v>sel</v>
@@ -10168,7 +10168,7 @@
         <v>6.9036140000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="14">
       <c r="A8" s="29" t="str">
         <f>Biopax!$A14</f>
         <v>join</v>
@@ -10198,7 +10198,7 @@
         <v>9.8627450000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="14">
       <c r="A9" s="29" t="str">
         <f>Biopax!$A15</f>
         <v>joinRel</v>
@@ -10228,7 +10228,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="14">
       <c r="A10" s="29" t="str">
         <f>Biopax!$A16</f>
         <v>joinFilter</v>
@@ -10258,7 +10258,7 @@
         <v>10.657895</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="14">
       <c r="A11" s="29" t="str">
         <f>Biopax!$A17</f>
         <v>joinRe</v>
@@ -10288,7 +10288,7 @@
         <v>10.666667</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="14">
       <c r="A12" s="29" t="str">
         <f>Biopax!$A18</f>
         <v>joinReif</v>
@@ -10318,7 +10318,7 @@
         <v>66.676190000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="14">
       <c r="A13" s="29" t="str">
         <f>Biopax!$A19</f>
         <v>varPathC</v>
@@ -10348,7 +10348,7 @@
         <v>25.862745</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="14">
       <c r="A14" s="29" t="str">
         <f>Biopax!$A20</f>
         <v>varPath</v>
@@ -10378,7 +10378,7 @@
         <v>33.349592999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="14">
       <c r="A15" s="29" t="str">
         <f>Biopax!$A21</f>
         <v>2union</v>
@@ -10408,7 +10408,7 @@
         <v>19.73</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="14">
       <c r="A16" s="29" t="str">
         <f>Biopax!$A22</f>
         <v>2union1Nest</v>
@@ -10438,7 +10438,7 @@
         <v>11.644231</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="14">
       <c r="A17" s="29" t="str">
         <f>Biopax!$A23</f>
         <v>pway</v>
@@ -10468,7 +10468,7 @@
         <v>34.221238999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="14">
       <c r="A18" s="29" t="str">
         <f>Biopax!$A24</f>
         <v>grp</v>
@@ -10498,7 +10498,7 @@
         <v>23.847826000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="14">
       <c r="A19" s="29" t="str">
         <f>Biopax!$A25</f>
         <v>grpAg</v>
@@ -10528,7 +10528,7 @@
         <v>27.177569999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="14">
       <c r="A20" s="29" t="str">
         <f>Biopax!$A26</f>
         <v>mulGrpAg</v>
@@ -10558,7 +10558,7 @@
         <v>56.32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="14">
       <c r="A21" s="29" t="str">
         <f>Biopax!$A27</f>
         <v>nestAg</v>
@@ -10588,7 +10588,7 @@
         <v>24.944444000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="14">
       <c r="A22" s="29" t="str">
         <f>Biopax!$A28</f>
         <v>exist</v>
@@ -10618,7 +10618,7 @@
         <v>34.734693999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="14">
       <c r="A23" s="29" t="str">
         <f>Biopax!$A29</f>
         <v>existAg</v>
@@ -10648,7 +10648,7 @@
         <v>59.063063</v>
       </c>
     </row>
-    <row r="51" spans="3:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="51" spans="3:3" ht="14">
       <c r="C51" s="26" t="s">
         <v>50</v>
       </c>
@@ -10656,7 +10656,7 @@
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Re-running benchmarks after fixing virtuoso.ini parameters.
</commit_message>
<xml_diff>
--- a/results/gdb_benchmark_results.xlsx
+++ b/results/gdb_benchmark_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandizi/Documents/Work/RRes/events/2018_swat4ls/paper/Review 1/material/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandizi/Documents/Work/RRes/events/2018_swat4ls/paper/graphdb-benchmarks/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9D28C7-A3A9-CC42-ABA7-9EDD5C9D33C1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC076125-99FD-8946-A0B4-8FD1778DE0C4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1598,67 +1598,67 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>622.47959200000003</c:v>
+                  <c:v>635.39655200000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.548387</c:v>
+                  <c:v>2.7523810000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.877778000000006</c:v>
+                  <c:v>65.495050000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.025641</c:v>
+                  <c:v>34.888888999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.1818179999999998</c:v>
+                  <c:v>13.113402000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.6190479999999994</c:v>
+                  <c:v>9.0178569999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.4</c:v>
+                  <c:v>13.273585000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.5775860000000002</c:v>
+                  <c:v>12.103774</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.494624</c:v>
+                  <c:v>10.872548999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>373.79411800000003</c:v>
+                  <c:v>354.23636399999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.914894</c:v>
+                  <c:v>27.292452999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>89.483146000000005</c:v>
+                  <c:v>101.359551</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.308510999999999</c:v>
+                  <c:v>12.244444</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.049020000000001</c:v>
+                  <c:v>11.572917</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>38.512605000000001</c:v>
+                  <c:v>37.576923000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21.039216</c:v>
+                  <c:v>21.574256999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.666667</c:v>
+                  <c:v>27.890243999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>65.769912000000005</c:v>
+                  <c:v>63.888888999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>22.274509999999999</c:v>
+                  <c:v>23.043956000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30.904254999999999</c:v>
+                  <c:v>33.606060999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>51.344828</c:v>
+                  <c:v>54.091836999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1964,67 +1964,67 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>5543.3195880000003</c:v>
+                  <c:v>5657.0833329999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0206189999999999</c:v>
+                  <c:v>14.739129999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>546.69662900000003</c:v>
+                  <c:v>525.22881400000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92.782608999999994</c:v>
+                  <c:v>75.115043999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.6306310000000002</c:v>
+                  <c:v>5.1495329999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.0099009999999993</c:v>
+                  <c:v>9.5454550000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.393162</c:v>
+                  <c:v>27.116667</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.4</c:v>
+                  <c:v>10.641304</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.807338999999999</c:v>
+                  <c:v>11.558824</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>60.181818</c:v>
+                  <c:v>56.190083000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25.590909</c:v>
+                  <c:v>24.934578999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.135922000000001</c:v>
+                  <c:v>18.756757</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.383838000000001</c:v>
+                  <c:v>14.120879</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.75</c:v>
+                  <c:v>12.936842</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.090909000000003</c:v>
+                  <c:v>39.484211000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26.521277000000001</c:v>
+                  <c:v>29.058824000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30.169643000000001</c:v>
+                  <c:v>29.875</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>83.12</c:v>
+                  <c:v>83.141176000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26.955752</c:v>
+                  <c:v>27.145833</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36.989691000000001</c:v>
+                  <c:v>42.930233000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>62.617283999999998</c:v>
+                  <c:v>58.055556000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2330,67 +2330,67 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>14721.444444000001</c:v>
+                  <c:v>13882.068375999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.847826</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1401.9534880000001</c:v>
+                  <c:v>1339.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.835052</c:v>
+                  <c:v>96.096153999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.9036140000000001</c:v>
+                  <c:v>6.6354170000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.8627450000000003</c:v>
+                  <c:v>8.4952380000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.5</c:v>
+                  <c:v>36.216495000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.657895</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.666667</c:v>
+                  <c:v>9.9529409999999991</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66.676190000000005</c:v>
+                  <c:v>48.666666999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25.862745</c:v>
+                  <c:v>25.133333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>33.349592999999999</c:v>
+                  <c:v>33.189473999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.73</c:v>
+                  <c:v>18.585366</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.644231</c:v>
+                  <c:v>11.444444000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34.221238999999997</c:v>
+                  <c:v>34.083333000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23.847826000000001</c:v>
+                  <c:v>22.330579</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>27.177569999999999</c:v>
+                  <c:v>26.28866</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>56.32</c:v>
+                  <c:v>48.085470000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24.944444000000001</c:v>
+                  <c:v>23.509091000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34.734693999999998</c:v>
+                  <c:v>28.373736999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>59.063063</c:v>
+                  <c:v>74.117647000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2994,67 +2994,67 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>622.47959200000003</c:v>
+                  <c:v>635.39655200000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.548387</c:v>
+                  <c:v>2.7523810000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.877778000000006</c:v>
+                  <c:v>65.495050000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.025641</c:v>
+                  <c:v>34.888888999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.1818179999999998</c:v>
+                  <c:v>13.113402000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.6190479999999994</c:v>
+                  <c:v>9.0178569999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.4</c:v>
+                  <c:v>13.273585000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.5775860000000002</c:v>
+                  <c:v>12.103774</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.494624</c:v>
+                  <c:v>10.872548999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>373.79411800000003</c:v>
+                  <c:v>354.23636399999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.914894</c:v>
+                  <c:v>27.292452999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>89.483146000000005</c:v>
+                  <c:v>101.359551</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.308510999999999</c:v>
+                  <c:v>12.244444</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.049020000000001</c:v>
+                  <c:v>11.572917</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>38.512605000000001</c:v>
+                  <c:v>37.576923000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21.039216</c:v>
+                  <c:v>21.574256999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.666667</c:v>
+                  <c:v>27.890243999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>65.769912000000005</c:v>
+                  <c:v>63.888888999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>22.274509999999999</c:v>
+                  <c:v>23.043956000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30.904254999999999</c:v>
+                  <c:v>33.606060999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>51.344828</c:v>
+                  <c:v>54.091836999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3598,67 +3598,67 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>5543.3195880000003</c:v>
+                  <c:v>5657.0833329999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0206189999999999</c:v>
+                  <c:v>14.739129999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>546.69662900000003</c:v>
+                  <c:v>525.22881400000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92.782608999999994</c:v>
+                  <c:v>75.115043999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.6306310000000002</c:v>
+                  <c:v>5.1495329999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.0099009999999993</c:v>
+                  <c:v>9.5454550000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.393162</c:v>
+                  <c:v>27.116667</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.4</c:v>
+                  <c:v>10.641304</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.807338999999999</c:v>
+                  <c:v>11.558824</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>60.181818</c:v>
+                  <c:v>56.190083000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25.590909</c:v>
+                  <c:v>24.934578999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.135922000000001</c:v>
+                  <c:v>18.756757</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.383838000000001</c:v>
+                  <c:v>14.120879</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.75</c:v>
+                  <c:v>12.936842</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.090909000000003</c:v>
+                  <c:v>39.484211000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26.521277000000001</c:v>
+                  <c:v>29.058824000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30.169643000000001</c:v>
+                  <c:v>29.875</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>83.12</c:v>
+                  <c:v>83.141176000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26.955752</c:v>
+                  <c:v>27.145833</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36.989691000000001</c:v>
+                  <c:v>42.930233000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>62.617283999999998</c:v>
+                  <c:v>58.055556000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4202,67 +4202,67 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>14721.444444000001</c:v>
+                  <c:v>13882.068375999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.847826</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1401.9534880000001</c:v>
+                  <c:v>1339.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.835052</c:v>
+                  <c:v>96.096153999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.9036140000000001</c:v>
+                  <c:v>6.6354170000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.8627450000000003</c:v>
+                  <c:v>8.4952380000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.5</c:v>
+                  <c:v>36.216495000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.657895</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.666667</c:v>
+                  <c:v>9.9529409999999991</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66.676190000000005</c:v>
+                  <c:v>48.666666999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25.862745</c:v>
+                  <c:v>25.133333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>33.349592999999999</c:v>
+                  <c:v>33.189473999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.73</c:v>
+                  <c:v>18.585366</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.644231</c:v>
+                  <c:v>11.444444000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34.221238999999997</c:v>
+                  <c:v>34.083333000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23.847826000000001</c:v>
+                  <c:v>22.330579</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>27.177569999999999</c:v>
+                  <c:v>26.28866</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>56.32</c:v>
+                  <c:v>48.085470000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24.944444000000001</c:v>
+                  <c:v>23.509091000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34.734693999999998</c:v>
+                  <c:v>28.373736999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>59.063063</c:v>
+                  <c:v>74.117647000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8480,10 +8480,10 @@
   <dimension ref="A1:IV29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
@@ -8622,7 +8622,7 @@
         <v>4.9505E-2</v>
       </c>
       <c r="D9" s="14">
-        <v>622.47959200000003</v>
+        <v>635.39655200000004</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>15</v>
@@ -8639,7 +8639,7 @@
         <v>0.76</v>
       </c>
       <c r="D10" s="14">
-        <v>2.548387</v>
+        <v>2.7523810000000002</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
@@ -8654,7 +8654,7 @@
         <v>0.114286</v>
       </c>
       <c r="D11" s="14">
-        <v>64.877778000000006</v>
+        <v>65.495050000000006</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -8669,7 +8669,7 @@
         <v>1.6727270000000001</v>
       </c>
       <c r="D12" s="14">
-        <v>34.025641</v>
+        <v>34.888888999999999</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -8684,7 +8684,7 @@
         <v>0.31428600000000001</v>
       </c>
       <c r="D13" s="14">
-        <v>6.1818179999999998</v>
+        <v>13.113402000000001</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -8699,7 +8699,7 @@
         <v>1.0659339999999999</v>
       </c>
       <c r="D14" s="14">
-        <v>8.6190479999999994</v>
+        <v>9.0178569999999993</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -8714,7 +8714,7 @@
         <v>1.194175</v>
       </c>
       <c r="D15" s="16">
-        <v>13.4</v>
+        <v>13.273585000000001</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -8729,7 +8729,7 @@
         <v>3.7083330000000001</v>
       </c>
       <c r="D16" s="14">
-        <v>9.5775860000000002</v>
+        <v>12.103774</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -8744,7 +8744,7 @@
         <v>3.913043</v>
       </c>
       <c r="D17" s="14">
-        <v>10.494624</v>
+        <v>10.872548999999999</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -8759,7 +8759,7 @@
         <v>6.8415840000000001</v>
       </c>
       <c r="D18" s="14">
-        <v>373.79411800000003</v>
+        <v>354.23636399999998</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -8774,7 +8774,7 @@
         <v>0.61904800000000004</v>
       </c>
       <c r="D19" s="14">
-        <v>27.914894</v>
+        <v>27.292452999999998</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -8789,7 +8789,7 @@
         <v>5.1397849999999998</v>
       </c>
       <c r="D20" s="14">
-        <v>89.483146000000005</v>
+        <v>101.359551</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -8804,7 +8804,7 @@
         <v>11.172043</v>
       </c>
       <c r="D21" s="14">
-        <v>12.308510999999999</v>
+        <v>12.244444</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -8819,7 +8819,7 @@
         <v>30.958333</v>
       </c>
       <c r="D22" s="17">
-        <v>11.049020000000001</v>
+        <v>11.572917</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -8834,7 +8834,7 @@
         <v>4.9519229999999999</v>
       </c>
       <c r="D23" s="14">
-        <v>38.512605000000001</v>
+        <v>37.576923000000001</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -8849,7 +8849,7 @@
         <v>8.9894739999999995</v>
       </c>
       <c r="D24" s="14">
-        <v>21.039216</v>
+        <v>21.574256999999999</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -8864,7 +8864,7 @@
         <v>10.757009</v>
       </c>
       <c r="D25" s="14">
-        <v>23.666667</v>
+        <v>27.890243999999999</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -8879,7 +8879,7 @@
         <v>827</v>
       </c>
       <c r="D26" s="14">
-        <v>65.769912000000005</v>
+        <v>63.888888999999999</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -8894,7 +8894,7 @@
         <v>10.677083</v>
       </c>
       <c r="D27" s="17">
-        <v>22.274509999999999</v>
+        <v>23.043956000000001</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -8909,7 +8909,7 @@
         <v>31.053763</v>
       </c>
       <c r="D28" s="14">
-        <v>30.904254999999999</v>
+        <v>33.606060999999997</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -8924,7 +8924,7 @@
         <v>59.613208</v>
       </c>
       <c r="D29" s="14">
-        <v>51.344828</v>
+        <v>54.091836999999998</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -8950,10 +8950,10 @@
   <dimension ref="A1:IV29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
@@ -9093,7 +9093,7 @@
         <v>0.47169800000000001</v>
       </c>
       <c r="D9" s="14">
-        <v>5543.3195880000003</v>
+        <v>5657.0833329999996</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>15</v>
@@ -9110,7 +9110,7 @@
         <v>5.7818180000000003</v>
       </c>
       <c r="D10" s="14">
-        <v>5.0206189999999999</v>
+        <v>14.739129999999999</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
@@ -9125,7 +9125,7 @@
         <v>0.36274499999999998</v>
       </c>
       <c r="D11" s="14">
-        <v>546.69662900000003</v>
+        <v>525.22881400000006</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -9140,7 +9140,7 @@
         <v>6.8738739999999998</v>
       </c>
       <c r="D12" s="14">
-        <v>92.782608999999994</v>
+        <v>75.115043999999997</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -9155,7 +9155,7 @@
         <v>0.76087000000000005</v>
       </c>
       <c r="D13" s="14">
-        <v>4.6306310000000002</v>
+        <v>5.1495329999999999</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -9170,7 +9170,7 @@
         <v>1.448</v>
       </c>
       <c r="D14" s="14">
-        <v>9.0099009999999993</v>
+        <v>9.5454550000000005</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -9185,7 +9185,7 @@
         <v>1.8658539999999999</v>
       </c>
       <c r="D15" s="14">
-        <v>17.393162</v>
+        <v>27.116667</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -9200,7 +9200,7 @@
         <v>8.7522120000000001</v>
       </c>
       <c r="D16" s="16">
-        <v>10.4</v>
+        <v>10.641304</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -9215,7 +9215,7 @@
         <v>5.8192769999999996</v>
       </c>
       <c r="D17" s="14">
-        <v>18.807338999999999</v>
+        <v>11.558824</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -9230,7 +9230,7 @@
         <v>491.942857</v>
       </c>
       <c r="D18" s="14">
-        <v>60.181818</v>
+        <v>56.190083000000001</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -9245,7 +9245,7 @@
         <v>1.8921570000000001</v>
       </c>
       <c r="D19" s="14">
-        <v>25.590909</v>
+        <v>24.934578999999999</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -9260,7 +9260,7 @@
         <v>7.5833329999999997</v>
       </c>
       <c r="D20" s="14">
-        <v>18.135922000000001</v>
+        <v>18.756757</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -9275,7 +9275,7 @@
         <v>10.340206</v>
       </c>
       <c r="D21" s="14">
-        <v>12.383838000000001</v>
+        <v>14.120879</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -9290,7 +9290,7 @@
         <v>44.315789000000002</v>
       </c>
       <c r="D22" s="15">
-        <v>11.75</v>
+        <v>12.936842</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -9305,7 +9305,7 @@
         <v>11.361905</v>
       </c>
       <c r="D23" s="14">
-        <v>36.090909000000003</v>
+        <v>39.484211000000002</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -9320,7 +9320,7 @@
         <v>13.53012</v>
       </c>
       <c r="D24" s="14">
-        <v>26.521277000000001</v>
+        <v>29.058824000000001</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -9335,7 +9335,7 @@
         <v>19.221239000000001</v>
       </c>
       <c r="D25" s="14">
-        <v>30.169643000000001</v>
+        <v>29.875</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -9350,7 +9350,7 @@
         <v>753.010989</v>
       </c>
       <c r="D26" s="15">
-        <v>83.12</v>
+        <v>83.141176000000002</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -9365,7 +9365,7 @@
         <v>20.428571000000002</v>
       </c>
       <c r="D27" s="14">
-        <v>26.955752</v>
+        <v>27.145833</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -9380,7 +9380,7 @@
         <v>21.775281</v>
       </c>
       <c r="D28" s="14">
-        <v>36.989691000000001</v>
+        <v>42.930233000000001</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -9395,7 +9395,7 @@
         <v>25.355768999999999</v>
       </c>
       <c r="D29" s="14">
-        <v>62.617283999999998</v>
+        <v>58.055556000000003</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -9421,10 +9421,10 @@
   <dimension ref="A1:IV29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
@@ -9564,7 +9564,7 @@
         <v>0.70454499999999998</v>
       </c>
       <c r="D9" s="14">
-        <v>14721.444444000001</v>
+        <v>13882.068375999999</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>15</v>
@@ -9581,7 +9581,7 @@
         <v>6.5729170000000003</v>
       </c>
       <c r="D10" s="14">
-        <v>13.847826</v>
+        <v>4.5</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
@@ -9596,7 +9596,7 @@
         <v>0.655914</v>
       </c>
       <c r="D11" s="14">
-        <v>1401.9534880000001</v>
+        <v>1339.1</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -9611,7 +9611,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="14">
-        <v>100.835052</v>
+        <v>96.096153999999999</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -9626,7 +9626,7 @@
         <v>1.605769</v>
       </c>
       <c r="D13" s="14">
-        <v>6.9036140000000001</v>
+        <v>6.6354170000000003</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -9641,7 +9641,7 @@
         <v>1.535088</v>
       </c>
       <c r="D14" s="14">
-        <v>9.8627450000000003</v>
+        <v>8.4952380000000005</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -9656,7 +9656,7 @@
         <v>4.68</v>
       </c>
       <c r="D15" s="16">
-        <v>21.5</v>
+        <v>36.216495000000002</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -9671,7 +9671,7 @@
         <v>9.4180329999999994</v>
       </c>
       <c r="D16" s="14">
-        <v>10.657895</v>
+        <v>9.9</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -9686,7 +9686,7 @@
         <v>5.9545450000000004</v>
       </c>
       <c r="D17" s="14">
-        <v>10.666667</v>
+        <v>9.9529409999999991</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -9701,7 +9701,7 @@
         <v>14.741935</v>
       </c>
       <c r="D18" s="17">
-        <v>66.676190000000005</v>
+        <v>48.666666999999997</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -9716,7 +9716,7 @@
         <v>1.81</v>
       </c>
       <c r="D19" s="14">
-        <v>25.862745</v>
+        <v>25.133333</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -9731,7 +9731,7 @@
         <v>4.0416670000000003</v>
       </c>
       <c r="D20" s="14">
-        <v>33.349592999999999</v>
+        <v>33.189473999999997</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -9746,7 +9746,7 @@
         <v>12.25</v>
       </c>
       <c r="D21" s="15">
-        <v>19.73</v>
+        <v>18.585366</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -9761,7 +9761,7 @@
         <v>41.304761999999997</v>
       </c>
       <c r="D22" s="14">
-        <v>11.644231</v>
+        <v>11.444444000000001</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -9776,7 +9776,7 @@
         <v>8.3406590000000005</v>
       </c>
       <c r="D23" s="14">
-        <v>34.221238999999997</v>
+        <v>34.083333000000003</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -9791,7 +9791,7 @@
         <v>14.344086000000001</v>
       </c>
       <c r="D24" s="14">
-        <v>23.847826000000001</v>
+        <v>22.330579</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -9806,7 +9806,7 @@
         <v>18.600000000000001</v>
       </c>
       <c r="D25" s="17">
-        <v>27.177569999999999</v>
+        <v>26.28866</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -9821,7 +9821,7 @@
         <v>780.01851899999997</v>
       </c>
       <c r="D26" s="15">
-        <v>56.32</v>
+        <v>48.085470000000001</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -9836,7 +9836,7 @@
         <v>19.745097999999999</v>
       </c>
       <c r="D27" s="14">
-        <v>24.944444000000001</v>
+        <v>23.509091000000002</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -9851,7 +9851,7 @@
         <v>19.142856999999999</v>
       </c>
       <c r="D28" s="14">
-        <v>34.734693999999998</v>
+        <v>28.373736999999998</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -9866,7 +9866,7 @@
         <v>36.047618999999997</v>
       </c>
       <c r="D29" s="14">
-        <v>59.063063</v>
+        <v>74.117647000000005</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -10029,7 +10029,7 @@
       </c>
       <c r="C3" s="33">
         <f>Biopax!$D9</f>
-        <v>622.47959200000003</v>
+        <v>635.39655200000004</v>
       </c>
       <c r="D3" s="32">
         <f>Ara!$C9</f>
@@ -10037,7 +10037,7 @@
       </c>
       <c r="E3" s="33">
         <f>Ara!$D9</f>
-        <v>5543.3195880000003</v>
+        <v>5657.0833329999996</v>
       </c>
       <c r="F3" s="32">
         <f>Wheat!$C9</f>
@@ -10045,7 +10045,7 @@
       </c>
       <c r="G3" s="33">
         <f>Wheat!$D9</f>
-        <v>14721.444444000001</v>
+        <v>13882.068375999999</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14">
@@ -10059,7 +10059,7 @@
       </c>
       <c r="C4" s="33">
         <f>Biopax!$D10</f>
-        <v>2.548387</v>
+        <v>2.7523810000000002</v>
       </c>
       <c r="D4" s="32">
         <f>Ara!$C10</f>
@@ -10067,7 +10067,7 @@
       </c>
       <c r="E4" s="33">
         <f>Ara!$D10</f>
-        <v>5.0206189999999999</v>
+        <v>14.739129999999999</v>
       </c>
       <c r="F4" s="32">
         <f>Wheat!$C10</f>
@@ -10075,7 +10075,7 @@
       </c>
       <c r="G4" s="33">
         <f>Wheat!$D10</f>
-        <v>13.847826</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14">
@@ -10089,7 +10089,7 @@
       </c>
       <c r="C5" s="33">
         <f>Biopax!$D11</f>
-        <v>64.877778000000006</v>
+        <v>65.495050000000006</v>
       </c>
       <c r="D5" s="32">
         <f>Ara!$C11</f>
@@ -10097,7 +10097,7 @@
       </c>
       <c r="E5" s="33">
         <f>Ara!$D11</f>
-        <v>546.69662900000003</v>
+        <v>525.22881400000006</v>
       </c>
       <c r="F5" s="32">
         <f>Wheat!$C11</f>
@@ -10105,7 +10105,7 @@
       </c>
       <c r="G5" s="33">
         <f>Wheat!$D11</f>
-        <v>1401.9534880000001</v>
+        <v>1339.1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14">
@@ -10119,7 +10119,7 @@
       </c>
       <c r="C6" s="33">
         <f>Biopax!$D12</f>
-        <v>34.025641</v>
+        <v>34.888888999999999</v>
       </c>
       <c r="D6" s="32">
         <f>Ara!$C12</f>
@@ -10127,7 +10127,7 @@
       </c>
       <c r="E6" s="33">
         <f>Ara!$D12</f>
-        <v>92.782608999999994</v>
+        <v>75.115043999999997</v>
       </c>
       <c r="F6" s="32">
         <f>Wheat!$C12</f>
@@ -10135,7 +10135,7 @@
       </c>
       <c r="G6" s="33">
         <f>Wheat!$D12</f>
-        <v>100.835052</v>
+        <v>96.096153999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14">
@@ -10149,7 +10149,7 @@
       </c>
       <c r="C7" s="33">
         <f>Biopax!$D13</f>
-        <v>6.1818179999999998</v>
+        <v>13.113402000000001</v>
       </c>
       <c r="D7" s="32">
         <f>Ara!$C13</f>
@@ -10157,7 +10157,7 @@
       </c>
       <c r="E7" s="33">
         <f>Ara!$D13</f>
-        <v>4.6306310000000002</v>
+        <v>5.1495329999999999</v>
       </c>
       <c r="F7" s="32">
         <f>Wheat!$C13</f>
@@ -10165,7 +10165,7 @@
       </c>
       <c r="G7" s="33">
         <f>Wheat!$D13</f>
-        <v>6.9036140000000001</v>
+        <v>6.6354170000000003</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14">
@@ -10179,7 +10179,7 @@
       </c>
       <c r="C8" s="33">
         <f>Biopax!$D14</f>
-        <v>8.6190479999999994</v>
+        <v>9.0178569999999993</v>
       </c>
       <c r="D8" s="32">
         <f>Ara!$C14</f>
@@ -10187,7 +10187,7 @@
       </c>
       <c r="E8" s="33">
         <f>Ara!$D14</f>
-        <v>9.0099009999999993</v>
+        <v>9.5454550000000005</v>
       </c>
       <c r="F8" s="32">
         <f>Wheat!$C14</f>
@@ -10195,7 +10195,7 @@
       </c>
       <c r="G8" s="33">
         <f>Wheat!$D14</f>
-        <v>9.8627450000000003</v>
+        <v>8.4952380000000005</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14">
@@ -10209,7 +10209,7 @@
       </c>
       <c r="C9" s="33">
         <f>Biopax!$D15</f>
-        <v>13.4</v>
+        <v>13.273585000000001</v>
       </c>
       <c r="D9" s="32">
         <f>Ara!$C15</f>
@@ -10217,7 +10217,7 @@
       </c>
       <c r="E9" s="33">
         <f>Ara!$D15</f>
-        <v>17.393162</v>
+        <v>27.116667</v>
       </c>
       <c r="F9" s="32">
         <f>Wheat!$C15</f>
@@ -10225,7 +10225,7 @@
       </c>
       <c r="G9" s="33">
         <f>Wheat!$D15</f>
-        <v>21.5</v>
+        <v>36.216495000000002</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14">
@@ -10239,7 +10239,7 @@
       </c>
       <c r="C10" s="33">
         <f>Biopax!$D16</f>
-        <v>9.5775860000000002</v>
+        <v>12.103774</v>
       </c>
       <c r="D10" s="32">
         <f>Ara!$C16</f>
@@ -10247,7 +10247,7 @@
       </c>
       <c r="E10" s="33">
         <f>Ara!$D16</f>
-        <v>10.4</v>
+        <v>10.641304</v>
       </c>
       <c r="F10" s="32">
         <f>Wheat!$C16</f>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="G10" s="33">
         <f>Wheat!$D16</f>
-        <v>10.657895</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14">
@@ -10269,7 +10269,7 @@
       </c>
       <c r="C11" s="33">
         <f>Biopax!$D17</f>
-        <v>10.494624</v>
+        <v>10.872548999999999</v>
       </c>
       <c r="D11" s="32">
         <f>Ara!$C17</f>
@@ -10277,7 +10277,7 @@
       </c>
       <c r="E11" s="33">
         <f>Ara!$D17</f>
-        <v>18.807338999999999</v>
+        <v>11.558824</v>
       </c>
       <c r="F11" s="32">
         <f>Wheat!$C17</f>
@@ -10285,7 +10285,7 @@
       </c>
       <c r="G11" s="33">
         <f>Wheat!$D17</f>
-        <v>10.666667</v>
+        <v>9.9529409999999991</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14">
@@ -10299,7 +10299,7 @@
       </c>
       <c r="C12" s="33">
         <f>Biopax!$D18</f>
-        <v>373.79411800000003</v>
+        <v>354.23636399999998</v>
       </c>
       <c r="D12" s="32">
         <f>Ara!$C18</f>
@@ -10307,7 +10307,7 @@
       </c>
       <c r="E12" s="33">
         <f>Ara!$D18</f>
-        <v>60.181818</v>
+        <v>56.190083000000001</v>
       </c>
       <c r="F12" s="32">
         <f>Wheat!$C18</f>
@@ -10315,7 +10315,7 @@
       </c>
       <c r="G12" s="33">
         <f>Wheat!$D18</f>
-        <v>66.676190000000005</v>
+        <v>48.666666999999997</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14">
@@ -10329,7 +10329,7 @@
       </c>
       <c r="C13" s="33">
         <f>Biopax!$D19</f>
-        <v>27.914894</v>
+        <v>27.292452999999998</v>
       </c>
       <c r="D13" s="32">
         <f>Ara!$C19</f>
@@ -10337,7 +10337,7 @@
       </c>
       <c r="E13" s="33">
         <f>Ara!$D19</f>
-        <v>25.590909</v>
+        <v>24.934578999999999</v>
       </c>
       <c r="F13" s="32">
         <f>Wheat!$C19</f>
@@ -10345,7 +10345,7 @@
       </c>
       <c r="G13" s="33">
         <f>Wheat!$D19</f>
-        <v>25.862745</v>
+        <v>25.133333</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14">
@@ -10359,7 +10359,7 @@
       </c>
       <c r="C14" s="33">
         <f>Biopax!$D20</f>
-        <v>89.483146000000005</v>
+        <v>101.359551</v>
       </c>
       <c r="D14" s="32">
         <f>Ara!$C20</f>
@@ -10367,7 +10367,7 @@
       </c>
       <c r="E14" s="33">
         <f>Ara!$D20</f>
-        <v>18.135922000000001</v>
+        <v>18.756757</v>
       </c>
       <c r="F14" s="32">
         <f>Wheat!$C20</f>
@@ -10375,7 +10375,7 @@
       </c>
       <c r="G14" s="33">
         <f>Wheat!$D20</f>
-        <v>33.349592999999999</v>
+        <v>33.189473999999997</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14">
@@ -10389,7 +10389,7 @@
       </c>
       <c r="C15" s="33">
         <f>Biopax!$D21</f>
-        <v>12.308510999999999</v>
+        <v>12.244444</v>
       </c>
       <c r="D15" s="32">
         <f>Ara!$C21</f>
@@ -10397,7 +10397,7 @@
       </c>
       <c r="E15" s="33">
         <f>Ara!$D21</f>
-        <v>12.383838000000001</v>
+        <v>14.120879</v>
       </c>
       <c r="F15" s="32">
         <f>Wheat!$C21</f>
@@ -10405,7 +10405,7 @@
       </c>
       <c r="G15" s="33">
         <f>Wheat!$D21</f>
-        <v>19.73</v>
+        <v>18.585366</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14">
@@ -10419,7 +10419,7 @@
       </c>
       <c r="C16" s="33">
         <f>Biopax!$D22</f>
-        <v>11.049020000000001</v>
+        <v>11.572917</v>
       </c>
       <c r="D16" s="32">
         <f>Ara!$C22</f>
@@ -10427,7 +10427,7 @@
       </c>
       <c r="E16" s="33">
         <f>Ara!$D22</f>
-        <v>11.75</v>
+        <v>12.936842</v>
       </c>
       <c r="F16" s="32">
         <f>Wheat!$C22</f>
@@ -10435,7 +10435,7 @@
       </c>
       <c r="G16" s="33">
         <f>Wheat!$D22</f>
-        <v>11.644231</v>
+        <v>11.444444000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14">
@@ -10449,7 +10449,7 @@
       </c>
       <c r="C17" s="33">
         <f>Biopax!$D23</f>
-        <v>38.512605000000001</v>
+        <v>37.576923000000001</v>
       </c>
       <c r="D17" s="32">
         <f>Ara!$C23</f>
@@ -10457,7 +10457,7 @@
       </c>
       <c r="E17" s="33">
         <f>Ara!$D23</f>
-        <v>36.090909000000003</v>
+        <v>39.484211000000002</v>
       </c>
       <c r="F17" s="32">
         <f>Wheat!$C23</f>
@@ -10465,7 +10465,7 @@
       </c>
       <c r="G17" s="33">
         <f>Wheat!$D23</f>
-        <v>34.221238999999997</v>
+        <v>34.083333000000003</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14">
@@ -10479,7 +10479,7 @@
       </c>
       <c r="C18" s="33">
         <f>Biopax!$D24</f>
-        <v>21.039216</v>
+        <v>21.574256999999999</v>
       </c>
       <c r="D18" s="32">
         <f>Ara!$C24</f>
@@ -10487,7 +10487,7 @@
       </c>
       <c r="E18" s="33">
         <f>Ara!$D24</f>
-        <v>26.521277000000001</v>
+        <v>29.058824000000001</v>
       </c>
       <c r="F18" s="32">
         <f>Wheat!$C24</f>
@@ -10495,7 +10495,7 @@
       </c>
       <c r="G18" s="33">
         <f>Wheat!$D24</f>
-        <v>23.847826000000001</v>
+        <v>22.330579</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14">
@@ -10509,7 +10509,7 @@
       </c>
       <c r="C19" s="33">
         <f>Biopax!$D25</f>
-        <v>23.666667</v>
+        <v>27.890243999999999</v>
       </c>
       <c r="D19" s="32">
         <f>Ara!$C25</f>
@@ -10517,7 +10517,7 @@
       </c>
       <c r="E19" s="33">
         <f>Ara!$D25</f>
-        <v>30.169643000000001</v>
+        <v>29.875</v>
       </c>
       <c r="F19" s="32">
         <f>Wheat!$C25</f>
@@ -10525,7 +10525,7 @@
       </c>
       <c r="G19" s="33">
         <f>Wheat!$D25</f>
-        <v>27.177569999999999</v>
+        <v>26.28866</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14">
@@ -10539,7 +10539,7 @@
       </c>
       <c r="C20" s="33">
         <f>Biopax!$D26</f>
-        <v>65.769912000000005</v>
+        <v>63.888888999999999</v>
       </c>
       <c r="D20" s="32">
         <f>Ara!$C26</f>
@@ -10547,7 +10547,7 @@
       </c>
       <c r="E20" s="33">
         <f>Ara!$D26</f>
-        <v>83.12</v>
+        <v>83.141176000000002</v>
       </c>
       <c r="F20" s="32">
         <f>Wheat!$C26</f>
@@ -10555,7 +10555,7 @@
       </c>
       <c r="G20" s="33">
         <f>Wheat!$D26</f>
-        <v>56.32</v>
+        <v>48.085470000000001</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14">
@@ -10569,7 +10569,7 @@
       </c>
       <c r="C21" s="33">
         <f>Biopax!$D27</f>
-        <v>22.274509999999999</v>
+        <v>23.043956000000001</v>
       </c>
       <c r="D21" s="32">
         <f>Ara!$C27</f>
@@ -10577,7 +10577,7 @@
       </c>
       <c r="E21" s="33">
         <f>Ara!$D27</f>
-        <v>26.955752</v>
+        <v>27.145833</v>
       </c>
       <c r="F21" s="32">
         <f>Wheat!$C27</f>
@@ -10585,7 +10585,7 @@
       </c>
       <c r="G21" s="33">
         <f>Wheat!$D27</f>
-        <v>24.944444000000001</v>
+        <v>23.509091000000002</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14">
@@ -10599,7 +10599,7 @@
       </c>
       <c r="C22" s="33">
         <f>Biopax!$D28</f>
-        <v>30.904254999999999</v>
+        <v>33.606060999999997</v>
       </c>
       <c r="D22" s="32">
         <f>Ara!$C28</f>
@@ -10607,7 +10607,7 @@
       </c>
       <c r="E22" s="33">
         <f>Ara!$D28</f>
-        <v>36.989691000000001</v>
+        <v>42.930233000000001</v>
       </c>
       <c r="F22" s="32">
         <f>Wheat!$C28</f>
@@ -10615,7 +10615,7 @@
       </c>
       <c r="G22" s="33">
         <f>Wheat!$D28</f>
-        <v>34.734693999999998</v>
+        <v>28.373736999999998</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14">
@@ -10629,7 +10629,7 @@
       </c>
       <c r="C23" s="33">
         <f>Biopax!$D29</f>
-        <v>51.344828</v>
+        <v>54.091836999999998</v>
       </c>
       <c r="D23" s="32">
         <f>Ara!$C29</f>
@@ -10637,7 +10637,7 @@
       </c>
       <c r="E23" s="33">
         <f>Ara!$D29</f>
-        <v>62.617283999999998</v>
+        <v>58.055556000000003</v>
       </c>
       <c r="F23" s="32">
         <f>Wheat!$C29</f>
@@ -10645,7 +10645,7 @@
       </c>
       <c r="G23" s="33">
         <f>Wheat!$D29</f>
-        <v>59.063063</v>
+        <v>74.117647000000005</v>
       </c>
     </row>
     <row r="51" spans="3:3" ht="14">

</xml_diff>

<commit_message>
Minimal change to charts.
</commit_message>
<xml_diff>
--- a/results/gdb_benchmark_results.xlsx
+++ b/results/gdb_benchmark_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandizi/Documents/Work/RRes/events/2018_swat4ls/paper/graphdb-benchmarks/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{320BB308-2D5E-E942-AC07-09DA8E1D6D74}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767AE418-82AD-714B-A70C-AD3662064970}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16960" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Biopax" sheetId="1" r:id="rId1"/>
@@ -3287,6 +3287,7 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -4260,6 +4261,7 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -5233,6 +5235,7 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -6206,6 +6209,7 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -7179,6 +7183,7 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -8152,6 +8157,7 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -15761,8 +15767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CD3143-BDBF-FD41-9A6E-2395CA27F127}">
   <dimension ref="A2:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView topLeftCell="A84" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16950,27 +16956,27 @@
         <v>52</v>
       </c>
       <c r="B25" s="24">
-        <f>AVERAGE(B3:B23)</f>
+        <f t="shared" ref="B25:G25" si="6">AVERAGE(B3:B23)</f>
         <v>48.598359142857149</v>
       </c>
       <c r="C25" s="24">
-        <f>AVERAGE(C3:C23)</f>
+        <f t="shared" si="6"/>
         <v>74.537711190476188</v>
       </c>
       <c r="D25" s="24">
-        <f>AVERAGE(D3:D23)</f>
+        <f t="shared" si="6"/>
         <v>69.185455428571416</v>
       </c>
       <c r="E25" s="24">
-        <f>AVERAGE(E3:E23)</f>
+        <f t="shared" si="6"/>
         <v>322.5146703333333</v>
       </c>
       <c r="F25" s="24">
-        <f>AVERAGE(F3:F23)</f>
+        <f t="shared" si="6"/>
         <v>48.072095857142855</v>
       </c>
       <c r="G25" s="24">
-        <f>AVERAGE(G3:G23)</f>
+        <f t="shared" si="6"/>
         <v>751.75106771428568</v>
       </c>
     </row>
@@ -16979,27 +16985,27 @@
         <v>51</v>
       </c>
       <c r="B26" s="24">
-        <f>AVERAGE(B7:B23)</f>
+        <f t="shared" ref="B26:G26" si="7">AVERAGE(B7:B23)</f>
         <v>59.880530823529412</v>
       </c>
       <c r="C26" s="24">
-        <f>AVERAGE(C7:C23)</f>
+        <f t="shared" si="7"/>
         <v>48.63288605882353</v>
       </c>
       <c r="D26" s="24">
-        <f>AVERAGE(D7:D23)</f>
+        <f t="shared" si="7"/>
         <v>84.670848764705866</v>
       </c>
       <c r="E26" s="24">
-        <f>AVERAGE(E7:E23)</f>
+        <f t="shared" si="7"/>
         <v>29.449515058823529</v>
       </c>
       <c r="F26" s="24">
-        <f>AVERAGE(F7:F23)</f>
+        <f t="shared" si="7"/>
         <v>58.445919823529415</v>
       </c>
       <c r="G26" s="24">
-        <f>AVERAGE(G7:G23)</f>
+        <f t="shared" si="7"/>
         <v>27.353405411764705</v>
       </c>
     </row>
@@ -17028,9 +17034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1244D381-3F4A-C741-9F71-32B4F873FC4E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>

</xml_diff>